<commit_message>
Adding stand affil for remaining non stand affil in 0-500 pubs.
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38BBA4E-6122-4A92-9227-CA9B67D68F7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905D9F50-24A7-4F83-B32E-E43DF445AC84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11081" uniqueCount="2288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11141" uniqueCount="2303">
   <si>
     <t>Country_stand</t>
   </si>
@@ -6889,13 +6889,58 @@
   </si>
   <si>
     <t>University of Gdansk - Institute of Oceanography</t>
+  </si>
+  <si>
+    <t>eCoast</t>
+  </si>
+  <si>
+    <t>University Centre in Svalbard (UNIS)</t>
+  </si>
+  <si>
+    <t>Instituto Oncologico Della Svizzera Italiana</t>
+  </si>
+  <si>
+    <t>Max-Planck-Institute für Ornithologie</t>
+  </si>
+  <si>
+    <t>Free University of Brussels (VUB) - Environmental Hydroacoustics Laboratory (EHL)</t>
+  </si>
+  <si>
+    <t>Simón Bolívar University - Centro de Biodiversidad Marina</t>
+  </si>
+  <si>
+    <t>University of Magallanes - Centro de Investigación GAIA Antártica</t>
+  </si>
+  <si>
+    <t>Villanova University - Department of Biology</t>
+  </si>
+  <si>
+    <t>Altenburg &amp; Wymenga ecological research and consultancy</t>
+  </si>
+  <si>
+    <t>University Malaysia Sabah - Borneo Marine Research Institute</t>
+  </si>
+  <si>
+    <t>National Institute of Polar Research</t>
+  </si>
+  <si>
+    <t>University of Gothenburg - Department of Marine Sciences</t>
+  </si>
+  <si>
+    <t>San Diego State University (SDSU) - Department of Anthropology</t>
+  </si>
+  <si>
+    <t>University of Kansas - Biodiversity Institute</t>
+  </si>
+  <si>
+    <t>Nelson Mandela University (NMU) - Department of Zoology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6913,6 +6958,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF343434"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -6944,11 +6996,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7263,10 +7318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2121"/>
+  <dimension ref="A1:AZ2136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1278" workbookViewId="0">
-      <selection activeCell="C1313" sqref="C1313"/>
+    <sheetView tabSelected="1" topLeftCell="A2117" workbookViewId="0">
+      <selection activeCell="E2137" sqref="E2137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -71266,6 +71321,216 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2122" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2122" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C2122" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D2122" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2122" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2123" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2123" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C2123" s="4" t="s">
+        <v>2289</v>
+      </c>
+      <c r="D2123" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2123" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2124" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2124" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C2124" t="s">
+        <v>2290</v>
+      </c>
+      <c r="D2124" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2125" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2125" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2125" t="s">
+        <v>2291</v>
+      </c>
+      <c r="D2125" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2125" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2126" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2126" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2126" t="s">
+        <v>2292</v>
+      </c>
+      <c r="D2126" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2126" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2127" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2127" t="s">
+        <v>2276</v>
+      </c>
+      <c r="C2127" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D2127" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2128" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2128" t="s">
+        <v>452</v>
+      </c>
+      <c r="C2128" t="s">
+        <v>2294</v>
+      </c>
+      <c r="D2128" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2128" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2129" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2129" t="s">
+        <v>2295</v>
+      </c>
+      <c r="D2129" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2129" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2130" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C2130" t="s">
+        <v>2296</v>
+      </c>
+      <c r="D2130" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2130" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2131" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C2131" t="s">
+        <v>2297</v>
+      </c>
+      <c r="D2131" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2131" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2132" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2132" t="s">
+        <v>2298</v>
+      </c>
+      <c r="D2132" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2132" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2133" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C2133" t="s">
+        <v>2299</v>
+      </c>
+      <c r="D2133" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2133" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2134" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2134" t="s">
+        <v>2300</v>
+      </c>
+      <c r="D2134" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2134" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2135" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2135" t="s">
+        <v>2301</v>
+      </c>
+      <c r="D2135" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2136" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C2136" t="s">
+        <v>2302</v>
+      </c>
+      <c r="D2136" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2136" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding stand affil for remaining non stand affil in 500-1000 pubs.
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905D9F50-24A7-4F83-B32E-E43DF445AC84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD2F89F-B322-4E18-BA9A-420148DC65A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11141" uniqueCount="2303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11229" uniqueCount="2325">
   <si>
     <t>Country_stand</t>
   </si>
@@ -6934,6 +6934,72 @@
   </si>
   <si>
     <t>Nelson Mandela University (NMU) - Department of Zoology</t>
+  </si>
+  <si>
+    <t>RMIT University</t>
+  </si>
+  <si>
+    <t>University of the Ryukyus - Graduate School of Engineering and Science</t>
+  </si>
+  <si>
+    <t>Forschungszentrum Jülich</t>
+  </si>
+  <si>
+    <t>Tohoku University - Graduate School of Agricultural Sciences - Laboratory Biological Oceanography</t>
+  </si>
+  <si>
+    <t>JAMSTEC (Japan Agency for Marine-Earth Science and Technology) - Research and Development Centre Submarine Resources</t>
+  </si>
+  <si>
+    <t>California Academy of Sciences - Invertebrate Zoology and Geology</t>
+  </si>
+  <si>
+    <t>Hiroshima University - Graduate School of Biosphere Science</t>
+  </si>
+  <si>
+    <t>Federal University of Pernambuco (UFPE) - Department of Biology - Laboratory Microbiology and Immunology</t>
+  </si>
+  <si>
+    <t>Ocean University of China - Key Lab Mariculture</t>
+  </si>
+  <si>
+    <t>University of Fribourg - Department of Geosciences</t>
+  </si>
+  <si>
+    <t>Sinop University - Faculty of Arts and Science - Department of Biology</t>
+  </si>
+  <si>
+    <t>Laboratory for Marine Fisheries Science and Food Production</t>
+  </si>
+  <si>
+    <t>University of Salamanca - Faculty of Geography and History - Department of Prehistory, Ancient History and Archaeology</t>
+  </si>
+  <si>
+    <t>Sant'Anna School of Advanced Studies - Institute of BioRobotics</t>
+  </si>
+  <si>
+    <t>University Leiden - Institute of Biology</t>
+  </si>
+  <si>
+    <t>Adam Mickiewicz University - Institute of Environmental Biology</t>
+  </si>
+  <si>
+    <t>Zoological Research Museum Alexander Koenig</t>
+  </si>
+  <si>
+    <t>National Taiwan Ocean University (NTOU) - Institute of Marine Biology</t>
+  </si>
+  <si>
+    <t>University of San Carlos - Department of Physics</t>
+  </si>
+  <si>
+    <t>Utrecht University</t>
+  </si>
+  <si>
+    <t>Mansoura University - Faculty of Sciences - Department of Geology</t>
+  </si>
+  <si>
+    <t>Chosun University - Department of Biology</t>
   </si>
 </sst>
 </file>
@@ -7318,10 +7384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2136"/>
+  <dimension ref="A1:AZ2158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2117" workbookViewId="0">
-      <selection activeCell="E2137" sqref="E2137"/>
+    <sheetView tabSelected="1" topLeftCell="A2148" workbookViewId="0">
+      <selection activeCell="C2159" sqref="C2159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -71531,6 +71597,314 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2137" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2137" t="s">
+        <v>2303</v>
+      </c>
+      <c r="D2137" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2137" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2138" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2138" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D2138" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2138" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2139" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2139" t="s">
+        <v>2305</v>
+      </c>
+      <c r="D2139" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2139" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2140" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2140" t="s">
+        <v>2306</v>
+      </c>
+      <c r="D2140" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2140" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2141" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2141" t="s">
+        <v>2307</v>
+      </c>
+      <c r="D2141" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2141" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2142" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2142" t="s">
+        <v>2308</v>
+      </c>
+      <c r="D2142" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2142" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2143" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2143" t="s">
+        <v>2309</v>
+      </c>
+      <c r="D2143" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2143" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2144" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2144" t="s">
+        <v>2310</v>
+      </c>
+      <c r="D2144" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2144" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2145" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2145" t="s">
+        <v>2311</v>
+      </c>
+      <c r="D2145" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2146" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C2146" t="s">
+        <v>2312</v>
+      </c>
+      <c r="D2146" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2146" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2147" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C2147" t="s">
+        <v>2313</v>
+      </c>
+      <c r="D2147" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2147" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2148" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2148" t="s">
+        <v>2314</v>
+      </c>
+      <c r="D2148" t="s">
+        <v>809</v>
+      </c>
+      <c r="E2148" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2149" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2149" t="s">
+        <v>2315</v>
+      </c>
+      <c r="D2149" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2149" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2150" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2150" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D2150" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2150" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2151" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C2151" t="s">
+        <v>2317</v>
+      </c>
+      <c r="D2151" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2151" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2152" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C2152" t="s">
+        <v>2318</v>
+      </c>
+      <c r="D2152" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2152" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2153" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2153" t="s">
+        <v>2319</v>
+      </c>
+      <c r="D2153" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2153" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2154" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C2154" t="s">
+        <v>2320</v>
+      </c>
+      <c r="D2154" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2154" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2155" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C2155" t="s">
+        <v>2321</v>
+      </c>
+      <c r="D2155" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2155" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2156" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C2156" t="s">
+        <v>2322</v>
+      </c>
+      <c r="D2156" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2156" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2157" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2157" t="s">
+        <v>2323</v>
+      </c>
+      <c r="D2157" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2157" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2158" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2158" t="s">
+        <v>2324</v>
+      </c>
+      <c r="D2158" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2158" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding stand affil for remaining non stand affil in 1000-1500 pubs.
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD2F89F-B322-4E18-BA9A-420148DC65A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5679E351-3A36-4B63-96FB-F0F6B8602494}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
   <sheets>
     <sheet name="Unique_Affiliations" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unique_Affiliations!$A$1:$AZ$2183</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11229" uniqueCount="2325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11357" uniqueCount="2357">
   <si>
     <t>Country_stand</t>
   </si>
@@ -7000,6 +7003,102 @@
   </si>
   <si>
     <t>Chosun University - Department of Biology</t>
+  </si>
+  <si>
+    <t>University of Guam - Marine Laboratory</t>
+  </si>
+  <si>
+    <t>Royal Albert Memorial Museum and Art Gallery</t>
+  </si>
+  <si>
+    <t>Museum of Nature and Archaeology</t>
+  </si>
+  <si>
+    <t>University of Liège - Faculty of Sciences - Department of Sciences and Management of the Environment - Laboratory of Fish Demography and Hydroecology</t>
+  </si>
+  <si>
+    <t>NOAA National Oceanic and Atmospheric Administration - Conservation Biology Division - Northwest Fisheries Science Center</t>
+  </si>
+  <si>
+    <t>Escuela Superior Politecnica del Litoral - Faculty of Life Sciences</t>
+  </si>
+  <si>
+    <t>ECOMAR Environmental Consultancy - Marine biology division</t>
+  </si>
+  <si>
+    <t>Kangwon National University - Department of Molecular Bioscience</t>
+  </si>
+  <si>
+    <t>State Oceanic Administration (SOA) - Lab of Satellite Ocean Environment Dynamics</t>
+  </si>
+  <si>
+    <t>Pukyong National University - Department of Marine Biology</t>
+  </si>
+  <si>
+    <t>University of Derby - Environmental Sustainability Research Centre</t>
+  </si>
+  <si>
+    <t>Catholic University of the North</t>
+  </si>
+  <si>
+    <t>University of the Ryukyus - Faculty of Science - Department of Chemistry, Biology, and Marine Science</t>
+  </si>
+  <si>
+    <t>University of Montpellier - Institut de biologie Computationnelle</t>
+  </si>
+  <si>
+    <t>Spanish Institute of Oceanography (IEO) - Centro Oceanografico de Vigo</t>
+  </si>
+  <si>
+    <t>CEI MAR Research Institute</t>
+  </si>
+  <si>
+    <t>German Center for Infection Research</t>
+  </si>
+  <si>
+    <t>Universidade Federal de Santa Catarina</t>
+  </si>
+  <si>
+    <t>Universiti Malaysia Terengganu (UMT) - Institute of Tropical Aquaculture</t>
+  </si>
+  <si>
+    <t>Syddansk Universitet - Department of Biology</t>
+  </si>
+  <si>
+    <t>University of Catania - Department Biological, Geological and Environmental Sciences</t>
+  </si>
+  <si>
+    <t>Royal Ontario Museum</t>
+  </si>
+  <si>
+    <t>Universitas Hasanuddin</t>
+  </si>
+  <si>
+    <t>Universidade Federal da Bahia</t>
+  </si>
+  <si>
+    <t>Consorzio Nazionale Interuniversitario per le Scienze del Mare (CoNISMa)</t>
+  </si>
+  <si>
+    <t>CSIR (Council for Scientific and Industrial Research) - National Institute of Oceanography (NIO)</t>
+  </si>
+  <si>
+    <t>Altai State University - Biology department</t>
+  </si>
+  <si>
+    <t>Colombia University - Department of Microbiology and Immunology</t>
+  </si>
+  <si>
+    <t>Autonomous University of Sinaloa - Faculty of Marine Sciences</t>
+  </si>
+  <si>
+    <t>Chonnam National University - Departement of Oceanography</t>
+  </si>
+  <si>
+    <t>IMOD (Instituto Científico Michael Owen Dillon)</t>
+  </si>
+  <si>
+    <t>University of Évora</t>
   </si>
 </sst>
 </file>
@@ -7384,10 +7483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2158"/>
+  <dimension ref="A1:AZ2190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2148" workbookViewId="0">
-      <selection activeCell="C2159" sqref="C2159"/>
+    <sheetView tabSelected="1" topLeftCell="A2171" workbookViewId="0">
+      <selection activeCell="C2191" sqref="C2191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -71905,7 +72004,456 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2159" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2159" t="s">
+        <v>2325</v>
+      </c>
+      <c r="D2159" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2159" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2160" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2160" t="s">
+        <v>2326</v>
+      </c>
+      <c r="D2160" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2160" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2161" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2161" t="s">
+        <v>2327</v>
+      </c>
+      <c r="D2161" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2161" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2162" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2162" t="s">
+        <v>2328</v>
+      </c>
+      <c r="D2162" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2162" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2163" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2163" t="s">
+        <v>2329</v>
+      </c>
+      <c r="D2163" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2163" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2164" t="s">
+        <v>597</v>
+      </c>
+      <c r="C2164" t="s">
+        <v>2330</v>
+      </c>
+      <c r="D2164" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2164" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2165" t="s">
+        <v>534</v>
+      </c>
+      <c r="C2165" t="s">
+        <v>2331</v>
+      </c>
+      <c r="D2165" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2165" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2166" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2166" t="s">
+        <v>2332</v>
+      </c>
+      <c r="D2166" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2166" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2167" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2167" t="s">
+        <v>2333</v>
+      </c>
+      <c r="D2167" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2167" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2168" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2168" t="s">
+        <v>2334</v>
+      </c>
+      <c r="D2168" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2168" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2169" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2169" t="s">
+        <v>2335</v>
+      </c>
+      <c r="D2169" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2169" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2170" t="s">
+        <v>452</v>
+      </c>
+      <c r="C2170" t="s">
+        <v>2336</v>
+      </c>
+      <c r="D2170" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2170" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2171" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2171" t="s">
+        <v>2337</v>
+      </c>
+      <c r="D2171" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2171" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2172" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2172" t="s">
+        <v>2338</v>
+      </c>
+      <c r="D2172" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2172" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2173" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2173" t="s">
+        <v>2339</v>
+      </c>
+      <c r="D2173" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2173" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2174" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2174" t="s">
+        <v>2340</v>
+      </c>
+      <c r="D2174" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2174" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2175" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2175" t="s">
+        <v>2341</v>
+      </c>
+      <c r="D2175" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2175" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2176" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2176" t="s">
+        <v>2342</v>
+      </c>
+      <c r="D2176" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2176" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2177" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2177" t="s">
+        <v>2343</v>
+      </c>
+      <c r="D2177" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2177" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2178" t="s">
+        <v>577</v>
+      </c>
+      <c r="C2178" t="s">
+        <v>2344</v>
+      </c>
+      <c r="D2178" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2178" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2179" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2179" t="s">
+        <v>2345</v>
+      </c>
+      <c r="D2179" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2179" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2180" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2180" t="s">
+        <v>2346</v>
+      </c>
+      <c r="D2180" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2180" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2181" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C2181" t="s">
+        <v>2347</v>
+      </c>
+      <c r="D2181" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2181" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2182" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2182" t="s">
+        <v>2348</v>
+      </c>
+      <c r="D2182" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2182" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2183" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2183" t="s">
+        <v>2349</v>
+      </c>
+      <c r="D2183" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2183" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2184" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2184" t="s">
+        <v>2350</v>
+      </c>
+      <c r="D2184" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2184" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2185" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C2185" t="s">
+        <v>2351</v>
+      </c>
+      <c r="D2185" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2185" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2186" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2186" t="s">
+        <v>2352</v>
+      </c>
+      <c r="D2186" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2186" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2187" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C2187" t="s">
+        <v>2353</v>
+      </c>
+      <c r="D2187" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2187" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2188" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2188" t="s">
+        <v>2354</v>
+      </c>
+      <c r="D2188" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2188" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2189" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C2189" t="s">
+        <v>2355</v>
+      </c>
+      <c r="D2189" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2189" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2190" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C2190" t="s">
+        <v>2356</v>
+      </c>
+      <c r="D2190" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2190" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:AZ2183" xr:uid="{5A62C1F1-D184-4829-823C-2AC85E221BFD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding stand affil for remaining non stand affil in 1500-2000 pubs.
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5679E351-3A36-4B63-96FB-F0F6B8602494}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29909BF4-5EF9-4FFA-B1AB-E3BECAFB25C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Unique_Affiliations" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unique_Affiliations!$A$1:$AZ$2183</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unique_Affiliations!$A$1:$AZ$2215</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11357" uniqueCount="2357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11494" uniqueCount="2394">
   <si>
     <t>Country_stand</t>
   </si>
@@ -7099,6 +7099,117 @@
   </si>
   <si>
     <t>University of Évora</t>
+  </si>
+  <si>
+    <t>RBINS Royal Belgian Institute of Natural Sciences (RBINS) - Belgian Marine Data Centre (BMDC)</t>
+  </si>
+  <si>
+    <t>Keio University - Department of Mathematics</t>
+  </si>
+  <si>
+    <t>University of Pisa - Department of Animal Pathology, Prophylaxis and Food Hygiene</t>
+  </si>
+  <si>
+    <t>Ghent University - Faculty of Sciences - Biology Department - Research Group Evolutionary morphology of vertebrates</t>
+  </si>
+  <si>
+    <t>University of Derby</t>
+  </si>
+  <si>
+    <t>Hong Kong University of Science and Technology</t>
+  </si>
+  <si>
+    <t>UFSCar - Federal University of São Carlos - Department of Ecology and Biological evolution</t>
+  </si>
+  <si>
+    <t>University of São Paulo (USP) - Institute of Oceanography</t>
+  </si>
+  <si>
+    <t>National Cancer Institute (NCI) - Laboratory of Cell and Developmental Signaling</t>
+  </si>
+  <si>
+    <t>Universidade Federal do Espírito Santo</t>
+  </si>
+  <si>
+    <t>U.S. Fish and Wildlife Service</t>
+  </si>
+  <si>
+    <t>Indonesian Institute of Science (LIPI)</t>
+  </si>
+  <si>
+    <t>California State Polytechnic University</t>
+  </si>
+  <si>
+    <t>Universidad Técnica de Manabí</t>
+  </si>
+  <si>
+    <t>University of Salamanca</t>
+  </si>
+  <si>
+    <t>Palau International Coral Reef Center</t>
+  </si>
+  <si>
+    <t>Palau</t>
+  </si>
+  <si>
+    <t>University of Girona (UdG)</t>
+  </si>
+  <si>
+    <t>Suez Canal University</t>
+  </si>
+  <si>
+    <t>Tohoku University</t>
+  </si>
+  <si>
+    <t>Université de Tunis El Manar</t>
+  </si>
+  <si>
+    <t>Tunesia</t>
+  </si>
+  <si>
+    <t>Ocean Conservancy</t>
+  </si>
+  <si>
+    <t>Shandong University</t>
+  </si>
+  <si>
+    <t>Brazil government - Ministry of education</t>
+  </si>
+  <si>
+    <t>Swiss Federal Institute of Technology</t>
+  </si>
+  <si>
+    <t>CK Genomics</t>
+  </si>
+  <si>
+    <t>ELIXIR Hub</t>
+  </si>
+  <si>
+    <t>Prince of Songkla University</t>
+  </si>
+  <si>
+    <t>National Marine Biodiversity Institute of Korea</t>
+  </si>
+  <si>
+    <t>Obafemi Awolowo University</t>
+  </si>
+  <si>
+    <t>Centre for Environmental Radioactivity (CERAD)</t>
+  </si>
+  <si>
+    <t>Sangmyung University</t>
+  </si>
+  <si>
+    <t>Orkney Islands Council Marine Services</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>Russian Federation - Commander Islands Biosphere Reserve</t>
+  </si>
+  <si>
+    <t>National University of the Littoral</t>
   </si>
 </sst>
 </file>
@@ -7483,10 +7594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2190"/>
+  <dimension ref="A1:AZ2224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2171" workbookViewId="0">
-      <selection activeCell="C2191" sqref="C2191"/>
+    <sheetView tabSelected="1" topLeftCell="A2216" workbookViewId="0">
+      <selection activeCell="C2224" sqref="C2224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72452,8 +72563,487 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2191" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2191" s="2" t="s">
+        <v>2357</v>
+      </c>
+      <c r="D2191" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2191" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2192" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2192" t="s">
+        <v>2358</v>
+      </c>
+      <c r="D2192" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2192" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2193" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2193" t="s">
+        <v>2359</v>
+      </c>
+      <c r="D2193" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2193" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2194" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2194" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2194" t="s">
+        <v>2360</v>
+      </c>
+      <c r="D2194" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2194" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2195" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2195" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D2195" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2195" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2196" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2196" t="s">
+        <v>2362</v>
+      </c>
+      <c r="D2196" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2196" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2197" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2197" t="s">
+        <v>2363</v>
+      </c>
+      <c r="D2197" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2197" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2198" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2198" t="s">
+        <v>2364</v>
+      </c>
+      <c r="D2198" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2198" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2199" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2199" t="s">
+        <v>2365</v>
+      </c>
+      <c r="D2199" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2199" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2200" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2200" t="s">
+        <v>2366</v>
+      </c>
+      <c r="D2200" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2200" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2201" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2201" t="s">
+        <v>2367</v>
+      </c>
+      <c r="D2201" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2201" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2202" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C2202" t="s">
+        <v>2368</v>
+      </c>
+      <c r="D2202" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2202" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2203" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2203" t="s">
+        <v>2369</v>
+      </c>
+      <c r="D2203" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2203" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2204" t="s">
+        <v>597</v>
+      </c>
+      <c r="C2204" t="s">
+        <v>2370</v>
+      </c>
+      <c r="D2204" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2204" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2205" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2205" t="s">
+        <v>2371</v>
+      </c>
+      <c r="D2205" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2205" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2206" t="s">
+        <v>2373</v>
+      </c>
+      <c r="C2206" t="s">
+        <v>2372</v>
+      </c>
+      <c r="D2206" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2206" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2207" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2207" t="s">
+        <v>2374</v>
+      </c>
+      <c r="D2207" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2207" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2208" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2208" t="s">
+        <v>2375</v>
+      </c>
+      <c r="D2208" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2208" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2209" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2209" t="s">
+        <v>2376</v>
+      </c>
+      <c r="D2209" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2209" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2210" t="s">
+        <v>2378</v>
+      </c>
+      <c r="C2210" t="s">
+        <v>2377</v>
+      </c>
+      <c r="D2210" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2210" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2211" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2211" t="s">
+        <v>2379</v>
+      </c>
+      <c r="D2211" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2211" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2212" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2212" t="s">
+        <v>2380</v>
+      </c>
+      <c r="D2212" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2212" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2213" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2213" t="s">
+        <v>2381</v>
+      </c>
+      <c r="D2213" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2213" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2214" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C2214" t="s">
+        <v>2382</v>
+      </c>
+      <c r="D2214" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2214" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2215" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2215" t="s">
+        <v>2383</v>
+      </c>
+      <c r="D2215" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2215" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2216" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2216" t="s">
+        <v>2384</v>
+      </c>
+      <c r="D2216" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2216" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2217" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C2217" t="s">
+        <v>2385</v>
+      </c>
+      <c r="D2217" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2217" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2218" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2218" t="s">
+        <v>2386</v>
+      </c>
+      <c r="D2218" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2218" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2219" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C2219" t="s">
+        <v>2387</v>
+      </c>
+      <c r="D2219" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2219" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2220" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C2220" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D2220" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2220" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2221" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2221" t="s">
+        <v>2389</v>
+      </c>
+      <c r="D2221" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2221" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2222" t="s">
+        <v>2391</v>
+      </c>
+      <c r="C2222" t="s">
+        <v>2390</v>
+      </c>
+      <c r="D2222" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2222" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2223" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C2223" t="s">
+        <v>2392</v>
+      </c>
+      <c r="D2223" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2223" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2224" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C2224" t="s">
+        <v>2393</v>
+      </c>
+      <c r="D2224" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2224" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AZ2183" xr:uid="{5A62C1F1-D184-4829-823C-2AC85E221BFD}"/>
+  <autoFilter ref="A1:AZ2215" xr:uid="{5A62C1F1-D184-4829-823C-2AC85E221BFD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding stand affil for remaining non stand affil in 2000-2500 pubs.
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29909BF4-5EF9-4FFA-B1AB-E3BECAFB25C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665AA761-5FA9-4026-8037-36182B1431A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11494" uniqueCount="2394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11626" uniqueCount="2430">
   <si>
     <t>Country_stand</t>
   </si>
@@ -7210,6 +7210,114 @@
   </si>
   <si>
     <t>National University of the Littoral</t>
+  </si>
+  <si>
+    <t>Hawaiʻi Institute of Marine Biology</t>
+  </si>
+  <si>
+    <t>Bahamas Marine Mammal Research Organization</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Lower Saxony Institute for Historical Coastal Research</t>
+  </si>
+  <si>
+    <t>Bharathidasan University</t>
+  </si>
+  <si>
+    <t>Ravenshaw University, Cuttack</t>
+  </si>
+  <si>
+    <t>Centro Universitario UAGro</t>
+  </si>
+  <si>
+    <t>Kuwait Institute for Scientific Research</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Museo de Historia Natural de El Salvador (MUHNES)</t>
+  </si>
+  <si>
+    <t>Universidad Peruana Cayetano Heredia</t>
+  </si>
+  <si>
+    <t>Escuela Superior Politecnica del Litoral</t>
+  </si>
+  <si>
+    <t>Rudjer Boskovic Institute</t>
+  </si>
+  <si>
+    <t>Recep Tayyip Erdoğan University</t>
+  </si>
+  <si>
+    <t>Kitasato University</t>
+  </si>
+  <si>
+    <t>Museo De Historia Natural Marina De Colombia</t>
+  </si>
+  <si>
+    <t>Northeastern University</t>
+  </si>
+  <si>
+    <t>University of Johannesburg</t>
+  </si>
+  <si>
+    <t>Yunnan University</t>
+  </si>
+  <si>
+    <t>Federal University of Santa Maria</t>
+  </si>
+  <si>
+    <t>Mangalore University</t>
+  </si>
+  <si>
+    <t>George Washington University</t>
+  </si>
+  <si>
+    <t>University of Nevada</t>
+  </si>
+  <si>
+    <t>Federal University of Minas Gerais</t>
+  </si>
+  <si>
+    <t>Autonomous University of Tamaulipas</t>
+  </si>
+  <si>
+    <t>Universidad Estatal a Distancia</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Al Azhar University</t>
+  </si>
+  <si>
+    <t>Universitatea Ovidius din Constanta</t>
+  </si>
+  <si>
+    <t>Uppsala University</t>
+  </si>
+  <si>
+    <t>Kütahya Dumlupınar University</t>
+  </si>
+  <si>
+    <t>Adam Mickiewicz University</t>
+  </si>
+  <si>
+    <t>Federal Institute Goiano</t>
+  </si>
+  <si>
+    <t>National Institute Of Oceanography and Fisheries</t>
+  </si>
+  <si>
+    <t>CICIMAR - Instituto Politécnico Nacional</t>
+  </si>
+  <si>
+    <t>Universiti Sains Malaysia</t>
   </si>
 </sst>
 </file>
@@ -7594,10 +7702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2224"/>
+  <dimension ref="A1:AZ2257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2216" workbookViewId="0">
-      <selection activeCell="C2224" sqref="C2224"/>
+    <sheetView tabSelected="1" topLeftCell="A2243" workbookViewId="0">
+      <selection activeCell="E2258" sqref="E2258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -73042,6 +73150,468 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2225" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2225" t="s">
+        <v>2394</v>
+      </c>
+      <c r="D2225" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2225" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2226" t="s">
+        <v>2396</v>
+      </c>
+      <c r="C2226" t="s">
+        <v>2395</v>
+      </c>
+      <c r="D2226" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2226" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2227" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2227" t="s">
+        <v>2397</v>
+      </c>
+      <c r="D2227" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2227" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2228" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2228" t="s">
+        <v>2398</v>
+      </c>
+      <c r="D2228" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2228" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2229" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2229" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D2229" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2229" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2230" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C2230" t="s">
+        <v>2400</v>
+      </c>
+      <c r="D2230" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2230" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2231" t="s">
+        <v>2402</v>
+      </c>
+      <c r="C2231" t="s">
+        <v>2401</v>
+      </c>
+      <c r="D2231" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2231" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2232" t="s">
+        <v>609</v>
+      </c>
+      <c r="C2232" t="s">
+        <v>2403</v>
+      </c>
+      <c r="D2232" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2232" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2233" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C2233" t="s">
+        <v>2404</v>
+      </c>
+      <c r="D2233" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2233" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2234" t="s">
+        <v>597</v>
+      </c>
+      <c r="C2234" t="s">
+        <v>2405</v>
+      </c>
+      <c r="D2234" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2234" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2235" t="s">
+        <v>554</v>
+      </c>
+      <c r="C2235" t="s">
+        <v>2406</v>
+      </c>
+      <c r="D2235" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2235" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2236" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C2236" t="s">
+        <v>2407</v>
+      </c>
+      <c r="D2236" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2236" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2237" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2237" t="s">
+        <v>2408</v>
+      </c>
+      <c r="D2237" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2237" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2238" t="s">
+        <v>534</v>
+      </c>
+      <c r="C2238" t="s">
+        <v>2409</v>
+      </c>
+      <c r="D2238" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2238" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2239" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2239" t="s">
+        <v>2410</v>
+      </c>
+      <c r="D2239" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2239" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2240" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C2240" t="s">
+        <v>2411</v>
+      </c>
+      <c r="D2240" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2240" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2241" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2241" t="s">
+        <v>2412</v>
+      </c>
+      <c r="D2241" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2241" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2242" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2242" t="s">
+        <v>2413</v>
+      </c>
+      <c r="D2242" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2242" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2243" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2243" t="s">
+        <v>2414</v>
+      </c>
+      <c r="D2243" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2243" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2244" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2244" t="s">
+        <v>2415</v>
+      </c>
+      <c r="D2244" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2244" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2245" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2245" t="s">
+        <v>2416</v>
+      </c>
+      <c r="D2245" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2245" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2246" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2246" t="s">
+        <v>2417</v>
+      </c>
+      <c r="D2246" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2246" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2247" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C2247" t="s">
+        <v>2418</v>
+      </c>
+      <c r="D2247" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2247" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2248" t="s">
+        <v>2420</v>
+      </c>
+      <c r="C2248" t="s">
+        <v>2419</v>
+      </c>
+      <c r="D2248" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2248" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2249" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2249" t="s">
+        <v>2421</v>
+      </c>
+      <c r="D2249" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2249" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2250" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C2250" t="s">
+        <v>2422</v>
+      </c>
+      <c r="D2250" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2250" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2251" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C2251" t="s">
+        <v>2423</v>
+      </c>
+      <c r="D2251" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2251" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2252" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C2252" t="s">
+        <v>2424</v>
+      </c>
+      <c r="D2252" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2252" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2253" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C2253" t="s">
+        <v>2425</v>
+      </c>
+      <c r="D2253" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2253" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2254" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2254" t="s">
+        <v>2426</v>
+      </c>
+      <c r="D2254" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2254" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2255" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2255" t="s">
+        <v>2427</v>
+      </c>
+      <c r="D2255" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2255" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2256" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C2256" t="s">
+        <v>2428</v>
+      </c>
+      <c r="D2256" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2256" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2257" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C2257" t="s">
+        <v>2429</v>
+      </c>
+      <c r="D2257" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2257" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AZ2215" xr:uid="{5A62C1F1-D184-4829-823C-2AC85E221BFD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding stand affil for remaining non stand affil in 2500-3000 pibs.
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665AA761-5FA9-4026-8037-36182B1431A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAF56CC-00E4-4171-BA45-4B1E060A365F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Unique_Affiliations" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unique_Affiliations!$A$1:$AZ$2215</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unique_Affiliations!$A$1:$AZ$2259</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11626" uniqueCount="2430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11790" uniqueCount="2473">
   <si>
     <t>Country_stand</t>
   </si>
@@ -7318,6 +7318,135 @@
   </si>
   <si>
     <t>Universiti Sains Malaysia</t>
+  </si>
+  <si>
+    <t>Kent State University at Stark</t>
+  </si>
+  <si>
+    <t>Fondazione CIMA</t>
+  </si>
+  <si>
+    <t>Nanyang Technological University</t>
+  </si>
+  <si>
+    <t>National Institute of Carpology (Gaertnerian Institution)</t>
+  </si>
+  <si>
+    <t>University of Chicago - Marine Biological Laboratory</t>
+  </si>
+  <si>
+    <t>Cairo Universiy</t>
+  </si>
+  <si>
+    <t>Jenness Enterprises</t>
+  </si>
+  <si>
+    <t>Rey Juan Carlos University</t>
+  </si>
+  <si>
+    <t>Gloucester Marine Genomics Institute</t>
+  </si>
+  <si>
+    <t>University of Adelaide</t>
+  </si>
+  <si>
+    <t>Eritrea Institute of Technology</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Kiel University (CAU) - Zoological museum</t>
+  </si>
+  <si>
+    <t>Geological Survey of Denmark and Greenland</t>
+  </si>
+  <si>
+    <t>State University of Londrina</t>
+  </si>
+  <si>
+    <t>Istanbul Technical University</t>
+  </si>
+  <si>
+    <t>Sungkyunkwan University</t>
+  </si>
+  <si>
+    <t>Free University of Berlin</t>
+  </si>
+  <si>
+    <t>Université d'Abomey Calavi</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>OBIS Ocean Biogeographic Information System - Deep Sea node</t>
+  </si>
+  <si>
+    <t>King's College London</t>
+  </si>
+  <si>
+    <t>Kumamoto University</t>
+  </si>
+  <si>
+    <t>Vietnam Academy of Science and Technology (VAST)</t>
+  </si>
+  <si>
+    <t>Indian Institute of Science Education and Research- Kolkata (IISERK)</t>
+  </si>
+  <si>
+    <t>National Marine Fisheries Research Institute of Poland</t>
+  </si>
+  <si>
+    <t>University of California - Riverside</t>
+  </si>
+  <si>
+    <t>Universidad de Los Lagos</t>
+  </si>
+  <si>
+    <t>Andhra University</t>
+  </si>
+  <si>
+    <t>MUSE (Museo delle Scienze)</t>
+  </si>
+  <si>
+    <t>Idaho State University</t>
+  </si>
+  <si>
+    <t>University Antilles Guyane</t>
+  </si>
+  <si>
+    <t>Kyungpook National University</t>
+  </si>
+  <si>
+    <t>Joetsu University of Education</t>
+  </si>
+  <si>
+    <t>Centre d'Écologie et des Sciences de la Conservation (CESCO)</t>
+  </si>
+  <si>
+    <t>University of Padua</t>
+  </si>
+  <si>
+    <t>Catholic University of Temuco</t>
+  </si>
+  <si>
+    <t>University of Bern</t>
+  </si>
+  <si>
+    <t>Nagoya University - University museum</t>
+  </si>
+  <si>
+    <t>Georgia Southern University</t>
+  </si>
+  <si>
+    <t>Purdue University</t>
+  </si>
+  <si>
+    <t>Coventry University</t>
+  </si>
+  <si>
+    <t>International Islamic University Malaysia</t>
   </si>
 </sst>
 </file>
@@ -7702,10 +7831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2257"/>
+  <dimension ref="A1:AZ2298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2243" workbookViewId="0">
-      <selection activeCell="E2258" sqref="E2258"/>
+    <sheetView tabSelected="1" topLeftCell="A2271" workbookViewId="0">
+      <selection activeCell="C2299" sqref="C2299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -73612,8 +73741,582 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2258" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2258" t="s">
+        <v>2430</v>
+      </c>
+      <c r="D2258" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2258" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2259" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2259" t="s">
+        <v>2431</v>
+      </c>
+      <c r="D2259" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2259" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2260" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C2260" t="s">
+        <v>2432</v>
+      </c>
+      <c r="D2260" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2260" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2261" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C2261" t="s">
+        <v>2433</v>
+      </c>
+      <c r="D2261" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2261" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2262" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2262" t="s">
+        <v>2434</v>
+      </c>
+      <c r="D2262" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2262" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2263" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2263" t="s">
+        <v>2435</v>
+      </c>
+      <c r="D2263" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2263" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2264" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2264" t="s">
+        <v>2436</v>
+      </c>
+      <c r="D2264" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2264" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2265" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2265" t="s">
+        <v>2437</v>
+      </c>
+      <c r="D2265" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2265" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2266" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2266" t="s">
+        <v>2438</v>
+      </c>
+      <c r="D2266" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2266" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2267" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2267" t="s">
+        <v>2439</v>
+      </c>
+      <c r="D2267" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2267" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2268" t="s">
+        <v>2441</v>
+      </c>
+      <c r="C2268" t="s">
+        <v>2440</v>
+      </c>
+      <c r="D2268" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2268" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2269" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2269" s="2" t="s">
+        <v>2442</v>
+      </c>
+      <c r="D2269" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2269" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2270" t="s">
+        <v>577</v>
+      </c>
+      <c r="C2270" t="s">
+        <v>2443</v>
+      </c>
+      <c r="D2270" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2270" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2271" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2271" t="s">
+        <v>2444</v>
+      </c>
+      <c r="D2271" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2271" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2272" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C2272" t="s">
+        <v>2445</v>
+      </c>
+      <c r="D2272" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2272" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2273" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2273" t="s">
+        <v>2446</v>
+      </c>
+      <c r="D2273" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2273" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2274" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2274" t="s">
+        <v>2447</v>
+      </c>
+      <c r="D2274" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2274" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2275" t="s">
+        <v>2449</v>
+      </c>
+      <c r="C2275" t="s">
+        <v>2448</v>
+      </c>
+      <c r="D2275" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2275" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2276" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2276" t="s">
+        <v>2450</v>
+      </c>
+      <c r="D2276" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2276" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2277" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2277" t="s">
+        <v>2451</v>
+      </c>
+      <c r="D2277" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2277" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2278" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2278" t="s">
+        <v>2452</v>
+      </c>
+      <c r="D2278" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2278" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2279" t="s">
+        <v>2283</v>
+      </c>
+      <c r="C2279" t="s">
+        <v>2453</v>
+      </c>
+      <c r="D2279" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2279" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2280" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2280" t="s">
+        <v>2454</v>
+      </c>
+      <c r="D2280" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2280" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2281" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C2281" t="s">
+        <v>2455</v>
+      </c>
+      <c r="D2281" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2281" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2282" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2282" s="2" t="s">
+        <v>2456</v>
+      </c>
+      <c r="D2282" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2282" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2283" t="s">
+        <v>452</v>
+      </c>
+      <c r="C2283" t="s">
+        <v>2457</v>
+      </c>
+      <c r="D2283" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2283" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2284" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2284" t="s">
+        <v>2458</v>
+      </c>
+      <c r="D2284" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2284" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2285" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2285" t="s">
+        <v>2459</v>
+      </c>
+      <c r="D2285" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2285" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2286" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2286" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D2286" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2286" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2287" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2287" t="s">
+        <v>2461</v>
+      </c>
+      <c r="D2287" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2287" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2288" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2288" t="s">
+        <v>2462</v>
+      </c>
+      <c r="D2288" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2288" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2289" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2289" t="s">
+        <v>2463</v>
+      </c>
+      <c r="D2289" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2289" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2290" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2290" t="s">
+        <v>2464</v>
+      </c>
+      <c r="D2290" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2290" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2291" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2291" t="s">
+        <v>2465</v>
+      </c>
+      <c r="D2291" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2291" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2292" t="s">
+        <v>452</v>
+      </c>
+      <c r="C2292" t="s">
+        <v>2466</v>
+      </c>
+      <c r="D2292" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2292" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2293" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2293" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C2293" t="s">
+        <v>2467</v>
+      </c>
+      <c r="D2293" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2293" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2294" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2294" t="s">
+        <v>2468</v>
+      </c>
+      <c r="D2294" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2294" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2295" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2295" t="s">
+        <v>2469</v>
+      </c>
+      <c r="D2295" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2295" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2296" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2296" t="s">
+        <v>2470</v>
+      </c>
+      <c r="D2296" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2296" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2297" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2297" t="s">
+        <v>2471</v>
+      </c>
+      <c r="D2297" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2297" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2298" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C2298" t="s">
+        <v>2472</v>
+      </c>
+      <c r="D2298" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2298" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AZ2215" xr:uid="{5A62C1F1-D184-4829-823C-2AC85E221BFD}"/>
+  <autoFilter ref="A1:AZ2259" xr:uid="{5A62C1F1-D184-4829-823C-2AC85E221BFD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding stand affil for remaining non stand affil in 3000-3500 pibs.
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAF56CC-00E4-4171-BA45-4B1E060A365F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D890AB5B-C816-43F7-BE55-6B8F01C1ECF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11790" uniqueCount="2473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12036" uniqueCount="2532">
   <si>
     <t>Country_stand</t>
   </si>
@@ -7447,6 +7447,183 @@
   </si>
   <si>
     <t>International Islamic University Malaysia</t>
+  </si>
+  <si>
+    <t>Ghent University - WAVES research group</t>
+  </si>
+  <si>
+    <t>Canadian Parks and Wilderness Society (CPAWS)</t>
+  </si>
+  <si>
+    <t>Blue Ventures</t>
+  </si>
+  <si>
+    <t>Golden Laboratories and Offices - National Renewable Energy Laboratory (NREL)</t>
+  </si>
+  <si>
+    <t>Birkbeck, University of London</t>
+  </si>
+  <si>
+    <t>Ecofys UK Ltd</t>
+  </si>
+  <si>
+    <t>Grantham Research Institute on Climate Change and the Environment</t>
+  </si>
+  <si>
+    <t>Franklin &amp; Marshall College</t>
+  </si>
+  <si>
+    <t>University of Savoy Mont Blanc - Chambery</t>
+  </si>
+  <si>
+    <t>Auckland War Memorial Museum</t>
+  </si>
+  <si>
+    <t>Carl von Ossietzky University of Oldenburg - ICBM</t>
+  </si>
+  <si>
+    <t>Chinese Academy of Sciences - Minististry of Agriculture - Inst Hydrobiol - Key Lab Freshwater Ecol &amp; Biotechnol</t>
+  </si>
+  <si>
+    <t>Chinese Academy of Sciences - Key Lab Aquat Bot &amp; Watershed Ecol</t>
+  </si>
+  <si>
+    <t>Ege University - Faculty of Fisheries</t>
+  </si>
+  <si>
+    <t>Instituto Politécnico Nacional - Center for Research and Advanced Studies</t>
+  </si>
+  <si>
+    <t>Instituto Politécnico Nacional - Center for Marine Sciences</t>
+  </si>
+  <si>
+    <t>Montana State University</t>
+  </si>
+  <si>
+    <t>Nanjing Agricultural University</t>
+  </si>
+  <si>
+    <t>National Research Council (CNR) - Institute of Geoscience &amp; Earth resources</t>
+  </si>
+  <si>
+    <t>Norwegian Institute for Water Research (NIVA)</t>
+  </si>
+  <si>
+    <t>Norwegian Polar Institute</t>
+  </si>
+  <si>
+    <t>Seagrass Ocean Rescue</t>
+  </si>
+  <si>
+    <t>Universitas Sam Ratulangi</t>
+  </si>
+  <si>
+    <t>Shanghai Jiao Tong University</t>
+  </si>
+  <si>
+    <t>St. Petersburg State University - Lab Macroecol &amp; Biogeog Invertebrates</t>
+  </si>
+  <si>
+    <t>University of Birmingham</t>
+  </si>
+  <si>
+    <t>University of California, Irvine</t>
+  </si>
+  <si>
+    <t>University of Hawaii - Institute of Marine Biology</t>
+  </si>
+  <si>
+    <t>University of Stavanger</t>
+  </si>
+  <si>
+    <t>University of Urbino</t>
+  </si>
+  <si>
+    <t>Virginia Commonwealth University</t>
+  </si>
+  <si>
+    <t>Zhejiang University of Technology</t>
+  </si>
+  <si>
+    <t>University of Santiago de Cali</t>
+  </si>
+  <si>
+    <t>Universidad de Oriente Venezuela</t>
+  </si>
+  <si>
+    <t>Miyazaki University Kibana Campus</t>
+  </si>
+  <si>
+    <t>University of KwaZulu-Natal</t>
+  </si>
+  <si>
+    <t>University of Koblenz and Landau</t>
+  </si>
+  <si>
+    <t>University of Isfahan</t>
+  </si>
+  <si>
+    <t>University of Huelva</t>
+  </si>
+  <si>
+    <t>Federal University of Mato Grosso</t>
+  </si>
+  <si>
+    <t>University of Chittagong</t>
+  </si>
+  <si>
+    <t>University of Calicut</t>
+  </si>
+  <si>
+    <t>Middlebury College</t>
+  </si>
+  <si>
+    <t>Michigan Sea Grant</t>
+  </si>
+  <si>
+    <t>Meguro Parasitological Museum</t>
+  </si>
+  <si>
+    <t>Massey University</t>
+  </si>
+  <si>
+    <t>Massachusetts Maritime Academy</t>
+  </si>
+  <si>
+    <t>Mediterrean House for Human Sciences</t>
+  </si>
+  <si>
+    <t>Luxembourg Institute of Science and Technology (LIST)</t>
+  </si>
+  <si>
+    <t>Lake Erie College of Osteopathic Medicine (LECOM)</t>
+  </si>
+  <si>
+    <t>Japan Atomic Energy Agency</t>
+  </si>
+  <si>
+    <t>Indiana University Bloomington</t>
+  </si>
+  <si>
+    <t>Instituto Nacional de Investigación y Desarrollo Pesquero (INIDEP)</t>
+  </si>
+  <si>
+    <t>Swiss Federal Institute of Technology Lausanne</t>
+  </si>
+  <si>
+    <t>Bogor Agricultural University</t>
+  </si>
+  <si>
+    <t>Birbal Sahni Institute of Palaeosciences</t>
+  </si>
+  <si>
+    <t>Academy of Scientific &amp; Innovative Research (AcSIR)</t>
+  </si>
+  <si>
+    <t>Ghent University - Faculty of Bioscience Engineering - Department of Data analytics and Mathematical modelling</t>
+  </si>
+  <si>
+    <t>National Institute for Amazon Research (INPA)</t>
   </si>
 </sst>
 </file>
@@ -7831,10 +8008,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2298"/>
+  <dimension ref="A1:AZ2359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2271" workbookViewId="0">
-      <selection activeCell="C2299" sqref="C2299"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2329" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2360" sqref="E2360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74315,6 +74493,866 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2299" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2299" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2299" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2299" t="s">
+        <v>2473</v>
+      </c>
+      <c r="D2299" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2299" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2300" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2300" t="s">
+        <v>2474</v>
+      </c>
+      <c r="D2300" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2300" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2301" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2301" t="s">
+        <v>2475</v>
+      </c>
+      <c r="D2301" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2301" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2302" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2302" t="s">
+        <v>2476</v>
+      </c>
+      <c r="D2302" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2302" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2303" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2303" t="s">
+        <v>2477</v>
+      </c>
+      <c r="D2303" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2303" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2304" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2304" t="s">
+        <v>2478</v>
+      </c>
+      <c r="D2304" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2304" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2305" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2305" t="s">
+        <v>2479</v>
+      </c>
+      <c r="D2305" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2305" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2306" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2306" t="s">
+        <v>2480</v>
+      </c>
+      <c r="D2306" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2306" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2307" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2307" t="s">
+        <v>2481</v>
+      </c>
+      <c r="D2307" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2307" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2308" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2308" t="s">
+        <v>2482</v>
+      </c>
+      <c r="D2308" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2308" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2309" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2309" s="2" t="s">
+        <v>2483</v>
+      </c>
+      <c r="D2309" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2309" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2310" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2310" t="s">
+        <v>2484</v>
+      </c>
+      <c r="D2310" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2310" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2311" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2311" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2311" t="s">
+        <v>2485</v>
+      </c>
+      <c r="D2311" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2311" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2312" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2312" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C2312" t="s">
+        <v>2486</v>
+      </c>
+      <c r="D2312" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2312" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2313" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2313" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2313" t="s">
+        <v>2487</v>
+      </c>
+      <c r="D2313" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2313" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2314" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2314" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D2314" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2314" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2315" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2315" t="s">
+        <v>2489</v>
+      </c>
+      <c r="D2315" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2315" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2316" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2316" t="s">
+        <v>2490</v>
+      </c>
+      <c r="D2316" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2316" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2317" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2317" t="s">
+        <v>2491</v>
+      </c>
+      <c r="D2317" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2317" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2318" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C2318" t="s">
+        <v>2492</v>
+      </c>
+      <c r="D2318" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2318" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2319" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C2319" t="s">
+        <v>2493</v>
+      </c>
+      <c r="D2319" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2319" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2320" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2320" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2320" t="s">
+        <v>2494</v>
+      </c>
+      <c r="D2320" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2320" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2321" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2321" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C2321" t="s">
+        <v>2495</v>
+      </c>
+      <c r="D2321" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2321" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2322" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2322" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2322" t="s">
+        <v>2496</v>
+      </c>
+      <c r="D2322" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2322" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2323" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2323" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C2323" t="s">
+        <v>2497</v>
+      </c>
+      <c r="D2323" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2323" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2324" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2324" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2324" t="s">
+        <v>2498</v>
+      </c>
+      <c r="D2324" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2324" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2325" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2325" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2325" t="s">
+        <v>2499</v>
+      </c>
+      <c r="D2325" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2325" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2326" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2326" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2326" t="s">
+        <v>2500</v>
+      </c>
+      <c r="D2326" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2326" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2327" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2327" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C2327" t="s">
+        <v>2501</v>
+      </c>
+      <c r="D2327" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2327" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2328" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2328" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2328" t="s">
+        <v>2502</v>
+      </c>
+      <c r="D2328" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2328" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2329" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2329" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2329" t="s">
+        <v>2503</v>
+      </c>
+      <c r="D2329" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2329" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2330" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2330" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2330" t="s">
+        <v>2504</v>
+      </c>
+      <c r="D2330" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2330" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2331" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2331" t="s">
+        <v>534</v>
+      </c>
+      <c r="C2331" t="s">
+        <v>2505</v>
+      </c>
+      <c r="D2331" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2331" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2332" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2332" t="s">
+        <v>2276</v>
+      </c>
+      <c r="C2332" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D2332" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2332" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2333" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2333" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2333" t="s">
+        <v>2507</v>
+      </c>
+      <c r="D2333" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2333" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2334" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2334" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C2334" t="s">
+        <v>2508</v>
+      </c>
+      <c r="D2334" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2334" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2335" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2335" t="s">
+        <v>2509</v>
+      </c>
+      <c r="D2335" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2335" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2336" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2336" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C2336" t="s">
+        <v>2510</v>
+      </c>
+      <c r="D2336" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2336" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2337" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2337" t="s">
+        <v>2511</v>
+      </c>
+      <c r="D2337" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2337" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2338" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2338" t="s">
+        <v>2512</v>
+      </c>
+      <c r="D2338" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2338" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2339" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2339" t="s">
+        <v>2513</v>
+      </c>
+      <c r="D2339" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2339" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2340" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2340" t="s">
+        <v>2514</v>
+      </c>
+      <c r="D2340" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2340" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2341" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2341" t="s">
+        <v>2515</v>
+      </c>
+      <c r="D2341" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2341" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2342" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2342" t="s">
+        <v>2516</v>
+      </c>
+      <c r="D2342" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2342" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2343" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2343" t="s">
+        <v>2517</v>
+      </c>
+      <c r="D2343" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2343" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2344" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C2344" t="s">
+        <v>2518</v>
+      </c>
+      <c r="D2344" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2344" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2345" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2345" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2345" t="s">
+        <v>2519</v>
+      </c>
+      <c r="D2345" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2345" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2346" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2346" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2346" t="s">
+        <v>2520</v>
+      </c>
+      <c r="D2346" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2346" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2347" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C2347" t="s">
+        <v>2521</v>
+      </c>
+      <c r="D2347" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2347" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2348" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2348" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2348" t="s">
+        <v>2522</v>
+      </c>
+      <c r="D2348" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2348" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2349" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C2349" t="s">
+        <v>1546</v>
+      </c>
+      <c r="D2349" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2349" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2350" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2350" t="s">
+        <v>2523</v>
+      </c>
+      <c r="D2350" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2350" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2351" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2351" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2351" t="s">
+        <v>2524</v>
+      </c>
+      <c r="D2351" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2351" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2352" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2352" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2352" t="s">
+        <v>2525</v>
+      </c>
+      <c r="D2352" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2352" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2353" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2353" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C2353" t="s">
+        <v>884</v>
+      </c>
+      <c r="D2353" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2353" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2354" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2354" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C2354" t="s">
+        <v>2526</v>
+      </c>
+      <c r="D2354" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2354" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2355" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2355" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C2355" t="s">
+        <v>2527</v>
+      </c>
+      <c r="D2355" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2355" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2356" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2356" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2356" t="s">
+        <v>2528</v>
+      </c>
+      <c r="D2356" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2356" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2357" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2357" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2357" t="s">
+        <v>2529</v>
+      </c>
+      <c r="D2357" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2357" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2358" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2358" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2358" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2358" t="s">
+        <v>2530</v>
+      </c>
+      <c r="D2358" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2358" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2359" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2359" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2359" t="s">
+        <v>2531</v>
+      </c>
+      <c r="D2359" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2359" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AZ2259" xr:uid="{5A62C1F1-D184-4829-823C-2AC85E221BFD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding stand affil for remaining non stand affil in 3500-4000 pibs.
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D890AB5B-C816-43F7-BE55-6B8F01C1ECF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2295B40-4D0B-44DB-BBBA-34103B395C87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12036" uniqueCount="2532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12274" uniqueCount="2593">
   <si>
     <t>Country_stand</t>
   </si>
@@ -7624,6 +7624,189 @@
   </si>
   <si>
     <t>National Institute for Amazon Research (INPA)</t>
+  </si>
+  <si>
+    <t>Drexel University - Academy of Natural Sciences</t>
+  </si>
+  <si>
+    <t>Alexandria University</t>
+  </si>
+  <si>
+    <t>Alexandru Ioan Cuza University</t>
+  </si>
+  <si>
+    <t>American University of Paris</t>
+  </si>
+  <si>
+    <t>Anadarko Colombia Company Sucursal Colombia</t>
+  </si>
+  <si>
+    <t>Bahrain Institute for Pearls &amp; Gemstones (DANAT)</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Kuroshio Biology Research Institute</t>
+  </si>
+  <si>
+    <t>Brown University</t>
+  </si>
+  <si>
+    <t>Cadi Ayyad University</t>
+  </si>
+  <si>
+    <t>City University of Hong Kong</t>
+  </si>
+  <si>
+    <t>Commonwealth Secretariat</t>
+  </si>
+  <si>
+    <t>Agricultural Research Center (ARC) - Plant Protection Research Institute (PPRI)</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Spanish Institute of Oceanography (IEO) - Centro Oceanografico de Gadiz</t>
+  </si>
+  <si>
+    <t>Czech University of Life Sciences</t>
+  </si>
+  <si>
+    <t>Danish Shellfish Center</t>
+  </si>
+  <si>
+    <t>Ghent University - Department of Civil Engineering</t>
+  </si>
+  <si>
+    <t>Ehime University</t>
+  </si>
+  <si>
+    <t>Environment and Climate Change Canada</t>
+  </si>
+  <si>
+    <t>University of Antwerp - Evolutionary Ecology Group</t>
+  </si>
+  <si>
+    <t>Ewha Womans University</t>
+  </si>
+  <si>
+    <t>Griffith University - Griffith Institute for Drug Discovery</t>
+  </si>
+  <si>
+    <t>Hohai University</t>
+  </si>
+  <si>
+    <t>Huazhong University of Science and Technology</t>
+  </si>
+  <si>
+    <t>Instituto Argentino de Investigación en Zonas Áridas (IADIZA)</t>
+  </si>
+  <si>
+    <t>Italian National Institute for Environmental Protection and Research (ISPRA)</t>
+  </si>
+  <si>
+    <t>Maurice Wilkins Centre for Molecular Biodiscovery</t>
+  </si>
+  <si>
+    <t>Minia University</t>
+  </si>
+  <si>
+    <t>Menoufia University</t>
+  </si>
+  <si>
+    <t>Nanjing Forestry University</t>
+  </si>
+  <si>
+    <t>Nanjing University</t>
+  </si>
+  <si>
+    <t>Natural History Museum and Institute</t>
+  </si>
+  <si>
+    <t>Newcastle University</t>
+  </si>
+  <si>
+    <t>Noakhali Science and Technology University</t>
+  </si>
+  <si>
+    <t>Novosibirsk State University (NSU)</t>
+  </si>
+  <si>
+    <t>Ondokuz Mayıs University</t>
+  </si>
+  <si>
+    <t>Oxford Brookes University</t>
+  </si>
+  <si>
+    <t>Soka University</t>
+  </si>
+  <si>
+    <t>Tunghai University</t>
+  </si>
+  <si>
+    <t>Unisinos (Universidade do Vale do Rio dos Sinos - Campus São Leopoldo)</t>
+  </si>
+  <si>
+    <t>University of the Balearic Islands</t>
+  </si>
+  <si>
+    <t>Côte d'Azur University</t>
+  </si>
+  <si>
+    <t>University of Cyprus</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Universiti Kebangsaan Malaysia</t>
+  </si>
+  <si>
+    <t>University of Lincoln</t>
+  </si>
+  <si>
+    <t>Universiti Malaysia Terengganu (UMT)</t>
+  </si>
+  <si>
+    <t>University of Mississippi</t>
+  </si>
+  <si>
+    <t>University of Toronto Scarborough</t>
+  </si>
+  <si>
+    <t>University of Toronto</t>
+  </si>
+  <si>
+    <t>UCLouvain Saint-Louis Brussels</t>
+  </si>
+  <si>
+    <t>University of the South Pacific</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>University of Skövde</t>
+  </si>
+  <si>
+    <t>University of Rome</t>
+  </si>
+  <si>
+    <t>University of New Caledonia</t>
+  </si>
+  <si>
+    <t>University of Mons</t>
+  </si>
+  <si>
+    <t>Amazon Rural Federal University (UFRA)</t>
+  </si>
+  <si>
+    <t>Manaaki Whenua – Landcare Research</t>
+  </si>
+  <si>
+    <t>National Centre for Polar and Ocean Research (NCPOR)</t>
   </si>
 </sst>
 </file>
@@ -8008,11 +8191,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2359"/>
+  <dimension ref="A1:AZ2418"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2329" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2360" sqref="E2360"/>
+      <pane ySplit="1" topLeftCell="A2386" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2419" sqref="E2419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75353,6 +75536,838 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2360" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2360" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2360" t="s">
+        <v>2532</v>
+      </c>
+      <c r="D2360" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2360" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2361" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2361" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2361" t="s">
+        <v>2533</v>
+      </c>
+      <c r="D2361" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2361" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2362" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2362" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C2362" t="s">
+        <v>2534</v>
+      </c>
+      <c r="D2362" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2362" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2363" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2363" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2363" t="s">
+        <v>2535</v>
+      </c>
+      <c r="D2363" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2363" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2364" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2364" t="s">
+        <v>534</v>
+      </c>
+      <c r="C2364" t="s">
+        <v>2536</v>
+      </c>
+      <c r="D2364" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2364" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2365" t="s">
+        <v>2538</v>
+      </c>
+      <c r="C2365" t="s">
+        <v>2537</v>
+      </c>
+      <c r="D2365" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2365" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2366" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2366" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2366" t="s">
+        <v>2539</v>
+      </c>
+      <c r="D2366" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2366" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2367" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2367" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2367" t="s">
+        <v>2540</v>
+      </c>
+      <c r="D2367" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2367" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2368" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C2368" t="s">
+        <v>2541</v>
+      </c>
+      <c r="D2368" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2368" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2369" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2369" t="s">
+        <v>970</v>
+      </c>
+      <c r="C2369" t="s">
+        <v>2542</v>
+      </c>
+      <c r="D2369" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2369" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2370" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2370" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2370" t="s">
+        <v>2543</v>
+      </c>
+      <c r="D2370" t="s">
+        <v>870</v>
+      </c>
+      <c r="E2370" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2371" t="s">
+        <v>2545</v>
+      </c>
+      <c r="C2371" t="s">
+        <v>2544</v>
+      </c>
+      <c r="D2371" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2371" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2372" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2372" t="s">
+        <v>2546</v>
+      </c>
+      <c r="D2372" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2372" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2373" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2373" t="s">
+        <v>568</v>
+      </c>
+      <c r="C2373" t="s">
+        <v>2547</v>
+      </c>
+      <c r="D2373" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2373" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2374" t="s">
+        <v>577</v>
+      </c>
+      <c r="C2374" t="s">
+        <v>2548</v>
+      </c>
+      <c r="D2374" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2374" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2375" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2375" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2375" t="s">
+        <v>2549</v>
+      </c>
+      <c r="D2375" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2375" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2376" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2376" t="s">
+        <v>2550</v>
+      </c>
+      <c r="D2376" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2376" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2377" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2377" t="s">
+        <v>2551</v>
+      </c>
+      <c r="D2377" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2377" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2378" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2378" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2378" t="s">
+        <v>2552</v>
+      </c>
+      <c r="D2378" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2378" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2379" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2379" t="s">
+        <v>2553</v>
+      </c>
+      <c r="D2379" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2379" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2380" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2380" t="s">
+        <v>2554</v>
+      </c>
+      <c r="D2380" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2380" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2381" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2381" t="s">
+        <v>2555</v>
+      </c>
+      <c r="D2381" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2381" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2382" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2382" t="s">
+        <v>2556</v>
+      </c>
+      <c r="D2382" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2382" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2383" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2383" t="s">
+        <v>2557</v>
+      </c>
+      <c r="D2383" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2383" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2384" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2384" t="s">
+        <v>2558</v>
+      </c>
+      <c r="D2384" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2384" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2385" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2385" t="s">
+        <v>2559</v>
+      </c>
+      <c r="D2385" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2385" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2386" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2386" t="s">
+        <v>2560</v>
+      </c>
+      <c r="D2386" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2386" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2387" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2387" t="s">
+        <v>2561</v>
+      </c>
+      <c r="D2387" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2387" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2388" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2388" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D2388" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2388" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2389" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2389" t="s">
+        <v>2563</v>
+      </c>
+      <c r="D2389" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2389" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2390" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2390" t="s">
+        <v>2564</v>
+      </c>
+      <c r="D2390" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2390" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2391" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2391" t="s">
+        <v>2565</v>
+      </c>
+      <c r="D2391" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2391" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2392" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2392" t="s">
+        <v>2566</v>
+      </c>
+      <c r="D2392" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2392" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2393" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C2393" t="s">
+        <v>2567</v>
+      </c>
+      <c r="D2393" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2393" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2394" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C2394" t="s">
+        <v>2568</v>
+      </c>
+      <c r="D2394" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2394" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2395" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2395" t="s">
+        <v>2569</v>
+      </c>
+      <c r="D2395" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2395" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2396" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2396" t="s">
+        <v>2570</v>
+      </c>
+      <c r="D2396" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2396" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2397" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C2397" t="s">
+        <v>2571</v>
+      </c>
+      <c r="D2397" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2397" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2398" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2398" t="s">
+        <v>2572</v>
+      </c>
+      <c r="D2398" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2398" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2399" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2399" t="s">
+        <v>2573</v>
+      </c>
+      <c r="D2399" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2399" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2400" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2400" t="s">
+        <v>2574</v>
+      </c>
+      <c r="D2400" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2400" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2401" t="s">
+        <v>2576</v>
+      </c>
+      <c r="C2401" t="s">
+        <v>2575</v>
+      </c>
+      <c r="D2401" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2401" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2402" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C2402" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D2402" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2402" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2403" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C2403" t="s">
+        <v>2577</v>
+      </c>
+      <c r="D2403" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2403" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2404" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2404" t="s">
+        <v>2578</v>
+      </c>
+      <c r="D2404" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2404" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2405" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C2405" t="s">
+        <v>2579</v>
+      </c>
+      <c r="D2405" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2405" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2406" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2406" t="s">
+        <v>2580</v>
+      </c>
+      <c r="D2406" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2406" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2407" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2407" t="s">
+        <v>2581</v>
+      </c>
+      <c r="D2407" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2407" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2408" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2408" t="s">
+        <v>2582</v>
+      </c>
+      <c r="D2408" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2408" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2409" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2409" t="s">
+        <v>2583</v>
+      </c>
+      <c r="D2409" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2409" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2410" t="s">
+        <v>2585</v>
+      </c>
+      <c r="C2410" t="s">
+        <v>2584</v>
+      </c>
+      <c r="D2410" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2410" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2411" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C2411" t="s">
+        <v>2586</v>
+      </c>
+      <c r="D2411" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2411" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2412" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2412" t="s">
+        <v>2587</v>
+      </c>
+      <c r="D2412" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2412" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2413" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C2413" t="s">
+        <v>2588</v>
+      </c>
+      <c r="D2413" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2413" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2414" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2414" t="s">
+        <v>2589</v>
+      </c>
+      <c r="D2414" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2414" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2415" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2415" t="s">
+        <v>2590</v>
+      </c>
+      <c r="D2415" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2415" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2416" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C2416" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D2416" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2416" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2417" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C2417" t="s">
+        <v>2591</v>
+      </c>
+      <c r="D2417" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2417" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2418" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2418" t="s">
+        <v>2592</v>
+      </c>
+      <c r="D2418" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2418" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AZ2259" xr:uid="{5A62C1F1-D184-4829-823C-2AC85E221BFD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding stand affil for remaining non stand affil in 4000-4500 pibs.
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2295B40-4D0B-44DB-BBBA-34103B395C87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE16B39F-53A6-43D9-B596-1E02FD2E8FE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12274" uniqueCount="2593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12402" uniqueCount="2624">
   <si>
     <t>Country_stand</t>
   </si>
@@ -7807,6 +7807,99 @@
   </si>
   <si>
     <t>National Centre for Polar and Ocean Research (NCPOR)</t>
+  </si>
+  <si>
+    <t>National University of Loja</t>
+  </si>
+  <si>
+    <t>Universitat de Lleida</t>
+  </si>
+  <si>
+    <t>Universidad Juárez Autónoma de Tabasco</t>
+  </si>
+  <si>
+    <t>University of Houston</t>
+  </si>
+  <si>
+    <t>Universidad de Guayaquil (UG)</t>
+  </si>
+  <si>
+    <t>University of Florence</t>
+  </si>
+  <si>
+    <t>Federal University of Lavras (UFLA)</t>
+  </si>
+  <si>
+    <t>Universidade Estadual de Maringá</t>
+  </si>
+  <si>
+    <t>Universidad de Costa Rica (UCR)</t>
+  </si>
+  <si>
+    <t>The presidency of the University of Basra</t>
+  </si>
+  <si>
+    <t>Andrés Bello National University</t>
+  </si>
+  <si>
+    <t>Seaweed Co Blue Turtle Ltd</t>
+  </si>
+  <si>
+    <t>Southeast Asian Fisheries Development Center (SEAFDEC)</t>
+  </si>
+  <si>
+    <t>Sahmyook University</t>
+  </si>
+  <si>
+    <t>Peking University</t>
+  </si>
+  <si>
+    <t>University of Zadar - Odjel za geografiju / Department of Geography (Zadar)</t>
+  </si>
+  <si>
+    <t>Nagasaki University</t>
+  </si>
+  <si>
+    <t>Marine &amp; Environmental Research (MER) Lab</t>
+  </si>
+  <si>
+    <t>King Saud University</t>
+  </si>
+  <si>
+    <t>İskenderun Technical University ISTE</t>
+  </si>
+  <si>
+    <t>International Commission on Zoological Nomenclature (ICZN)</t>
+  </si>
+  <si>
+    <t>Gothenburg Global Biodiversity Centre</t>
+  </si>
+  <si>
+    <t>Girne American University</t>
+  </si>
+  <si>
+    <t>Fukuoka Institute of Health and Environmental Sciences</t>
+  </si>
+  <si>
+    <t>Dr. MGR Fisheries College and Research Institute</t>
+  </si>
+  <si>
+    <t>CIBIO – Research Centre in Biodiversity and Genetic Resources</t>
+  </si>
+  <si>
+    <t>Chinese Academy of Fishery Sciences</t>
+  </si>
+  <si>
+    <t>Carmel College of Arts, Science and Commerce for Women </t>
+  </si>
+  <si>
+    <t>Brawijaya University</t>
+  </si>
+  <si>
+    <t>Amgueddfa Cymru – National Museum Wales</t>
+  </si>
+  <si>
+    <t>Israel Oceanographic and Limnological Research (IOLR)</t>
   </si>
 </sst>
 </file>
@@ -8191,11 +8284,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2418"/>
+  <dimension ref="A1:AZ2450"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2386" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2419" sqref="E2419"/>
+      <pane ySplit="1" topLeftCell="A2425" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2451" sqref="C2451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76368,6 +76461,454 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2419" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2419" t="s">
+        <v>597</v>
+      </c>
+      <c r="C2419" t="s">
+        <v>2593</v>
+      </c>
+      <c r="D2419" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2419" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2420" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2420" t="s">
+        <v>2594</v>
+      </c>
+      <c r="D2420" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2420" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2421" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C2421" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D2421" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2421" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2422" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2422" t="s">
+        <v>2596</v>
+      </c>
+      <c r="D2422" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2422" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2423" t="s">
+        <v>597</v>
+      </c>
+      <c r="C2423" t="s">
+        <v>2597</v>
+      </c>
+      <c r="D2423" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2423" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2424" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2424" t="s">
+        <v>2598</v>
+      </c>
+      <c r="D2424" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2424" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2425" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2425" t="s">
+        <v>2599</v>
+      </c>
+      <c r="D2425" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2425" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2426" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2426" t="s">
+        <v>2600</v>
+      </c>
+      <c r="D2426" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2426" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2427" t="s">
+        <v>2420</v>
+      </c>
+      <c r="C2427" t="s">
+        <v>2601</v>
+      </c>
+      <c r="D2427" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2427" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2428" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C2428" t="s">
+        <v>2602</v>
+      </c>
+      <c r="D2428" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2428" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2429" t="s">
+        <v>452</v>
+      </c>
+      <c r="C2429" t="s">
+        <v>2603</v>
+      </c>
+      <c r="D2429" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2429" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2430" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C2430" t="s">
+        <v>2604</v>
+      </c>
+      <c r="D2430" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2430" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2431" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C2431" t="s">
+        <v>2605</v>
+      </c>
+      <c r="D2431" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2431" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2432" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2432" t="s">
+        <v>2606</v>
+      </c>
+      <c r="D2432" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2432" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2433" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2433" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2433" t="s">
+        <v>716</v>
+      </c>
+      <c r="D2433" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2433" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2434" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2434" t="s">
+        <v>2607</v>
+      </c>
+      <c r="D2434" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2434" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2435" t="s">
+        <v>554</v>
+      </c>
+      <c r="C2435" t="s">
+        <v>2608</v>
+      </c>
+      <c r="D2435" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2435" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2436" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2436" t="s">
+        <v>2609</v>
+      </c>
+      <c r="D2436" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2436" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2437" t="s">
+        <v>2576</v>
+      </c>
+      <c r="C2437" t="s">
+        <v>2610</v>
+      </c>
+      <c r="D2437" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2437" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2438" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C2438" t="s">
+        <v>2611</v>
+      </c>
+      <c r="D2438" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2438" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2439" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C2439" t="s">
+        <v>2612</v>
+      </c>
+      <c r="D2439" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2439" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2440" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C2440" t="s">
+        <v>2613</v>
+      </c>
+      <c r="D2440" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2440" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2441" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C2441" t="s">
+        <v>2614</v>
+      </c>
+      <c r="D2441" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2441" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2442" t="s">
+        <v>2576</v>
+      </c>
+      <c r="C2442" t="s">
+        <v>2615</v>
+      </c>
+      <c r="D2442" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2442" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2443" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2443" t="s">
+        <v>2616</v>
+      </c>
+      <c r="D2443" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2443" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2444" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2444" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2444" t="s">
+        <v>2617</v>
+      </c>
+      <c r="D2444" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2444" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2445" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2445" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C2445" t="s">
+        <v>2618</v>
+      </c>
+      <c r="D2445" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2445" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2446" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2446" t="s">
+        <v>2619</v>
+      </c>
+      <c r="D2446" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2446" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2447" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2447" t="s">
+        <v>2620</v>
+      </c>
+      <c r="D2447" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2447" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2448" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C2448" t="s">
+        <v>2621</v>
+      </c>
+      <c r="D2448" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2448" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2449" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2449" t="s">
+        <v>2622</v>
+      </c>
+      <c r="D2449" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2449" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2450" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C2450" t="s">
+        <v>2623</v>
+      </c>
+      <c r="D2450" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2450" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AZ2259" xr:uid="{5A62C1F1-D184-4829-823C-2AC85E221BFD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding stand affil for remaining non stand affil in 4500-5000 pibs.
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE16B39F-53A6-43D9-B596-1E02FD2E8FE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AAECA8-38EB-48D7-8F65-6AB8388713FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12402" uniqueCount="2624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12471" uniqueCount="2641">
   <si>
     <t>Country_stand</t>
   </si>
@@ -7900,6 +7900,57 @@
   </si>
   <si>
     <t>Israel Oceanographic and Limnological Research (IOLR)</t>
+  </si>
+  <si>
+    <t>University of Zaragoza</t>
+  </si>
+  <si>
+    <t>University of Rwanda</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>University of Pretoria</t>
+  </si>
+  <si>
+    <t>University of Mostaghanem Central</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Netherlands Food and Consumer Product Safety Authority (NVWA)</t>
+  </si>
+  <si>
+    <t>Hawaii state government - Aquatic Resources Division</t>
+  </si>
+  <si>
+    <t>Nautilus Minerals Pacific Ltd</t>
+  </si>
+  <si>
+    <t>Loughborough University</t>
+  </si>
+  <si>
+    <t>Liverpool John Moores University</t>
+  </si>
+  <si>
+    <t>La Trobe University</t>
+  </si>
+  <si>
+    <t>Kaliningrad State Technical University</t>
+  </si>
+  <si>
+    <t>IFAPA center El Toruño</t>
+  </si>
+  <si>
+    <t>Ghent University - Faculty of Sciences</t>
+  </si>
+  <si>
+    <t>Chosun University</t>
+  </si>
+  <si>
+    <t>Boston University</t>
   </si>
 </sst>
 </file>
@@ -8284,11 +8335,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2450"/>
+  <dimension ref="A1:AZ2467"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2425" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2451" sqref="C2451"/>
+      <pane ySplit="1" topLeftCell="A2434" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2468" sqref="B2468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76909,6 +76960,247 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2451" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2451" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2451" t="s">
+        <v>2624</v>
+      </c>
+      <c r="D2451" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2451" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2452" t="s">
+        <v>2626</v>
+      </c>
+      <c r="C2452" t="s">
+        <v>2625</v>
+      </c>
+      <c r="D2452" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2452" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2453" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2453" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C2453" t="s">
+        <v>2627</v>
+      </c>
+      <c r="D2453" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2453" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2454" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2454" t="s">
+        <v>2629</v>
+      </c>
+      <c r="C2454" t="s">
+        <v>2628</v>
+      </c>
+      <c r="D2454" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2454" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2455" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2455" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C2455" t="s">
+        <v>2630</v>
+      </c>
+      <c r="D2455" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2455" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2456" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2456" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2456" t="s">
+        <v>2631</v>
+      </c>
+      <c r="D2456" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2456" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2457" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2457" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2457" t="s">
+        <v>2632</v>
+      </c>
+      <c r="D2457" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2457" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2458" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2458" t="s">
+        <v>933</v>
+      </c>
+      <c r="C2458" t="s">
+        <v>948</v>
+      </c>
+      <c r="D2458" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2458" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2459" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2459" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2459" t="s">
+        <v>2633</v>
+      </c>
+      <c r="D2459" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2459" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2460" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2460" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2460" t="s">
+        <v>2634</v>
+      </c>
+      <c r="D2460" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2460" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2461" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2461" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2461" t="s">
+        <v>2635</v>
+      </c>
+      <c r="D2461" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2461" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2462" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2462" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2462" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2462" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2462" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2463" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2463" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C2463" t="s">
+        <v>2636</v>
+      </c>
+      <c r="D2463" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2463" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2464" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2464" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2464" t="s">
+        <v>2637</v>
+      </c>
+      <c r="D2464" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2464" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2465" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2465" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2465" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2465" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="D2465" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2465" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2466" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2466" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2466" t="s">
+        <v>2639</v>
+      </c>
+      <c r="D2466" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2466" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2467" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2467" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2467" t="s">
+        <v>2640</v>
+      </c>
+      <c r="D2467" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2467" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AZ2259" xr:uid="{5A62C1F1-D184-4829-823C-2AC85E221BFD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding stand affil for remaining non stand affil from LW-data-systems.
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D15D16-EE33-4264-BD7A-CD7A1D9F2130}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CFDDA4-1EB8-4F03-BEB7-3F853A90FA91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Unique_Affiliations" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unique_Affiliations!$A$1:$AZ$2259</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unique_Affiliations!$A$1:$AZ$2527</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12479" uniqueCount="2643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12834" uniqueCount="2732">
   <si>
     <t>Country_stand</t>
   </si>
@@ -7957,6 +7957,273 @@
   </si>
   <si>
     <t>Université Libre de Bruxelles (ULB) - Acoustics and Environmental Hydroacoustics Lab</t>
+  </si>
+  <si>
+    <t>University of Manchester - Department of computer science</t>
+  </si>
+  <si>
+    <t>Manchester Interdisciplinary Biocentre - National Centre for Text Mining (NaCTeM)</t>
+  </si>
+  <si>
+    <t>eOceans</t>
+  </si>
+  <si>
+    <t>Australian National University - Research school of Earth Sciences</t>
+  </si>
+  <si>
+    <t>De Noordzee</t>
+  </si>
+  <si>
+    <t>Natuur En Milieu</t>
+  </si>
+  <si>
+    <t>European Space Agency</t>
+  </si>
+  <si>
+    <t>personal emailadres</t>
+  </si>
+  <si>
+    <t>personal interest</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Phillipines</t>
+  </si>
+  <si>
+    <t>strandvondsten.nl</t>
+  </si>
+  <si>
+    <t>crabdatabase.info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observation.org, </t>
+  </si>
+  <si>
+    <t>Brazilian Government, Ministry of Agriculture, Livestock and Food supply, Brazilian Agricultural Research Corporation</t>
+  </si>
+  <si>
+    <t>Research Foundation – Flanders</t>
+  </si>
+  <si>
+    <t>University of Liège - TERRA research centre</t>
+  </si>
+  <si>
+    <t>Bloomberg</t>
+  </si>
+  <si>
+    <t>Reuters</t>
+  </si>
+  <si>
+    <t>The New York Times</t>
+  </si>
+  <si>
+    <t>Open Street Map Foundation</t>
+  </si>
+  <si>
+    <t>Information system on Aquatic Non-Indigenous and Cryptogenic Species (AquaNIS)</t>
+  </si>
+  <si>
+    <t>MyDiveAlbum</t>
+  </si>
+  <si>
+    <t>Cyprus University of Technology</t>
+  </si>
+  <si>
+    <t>Indonesian Institute of Science</t>
+  </si>
+  <si>
+    <t>BGI-Qingdao</t>
+  </si>
+  <si>
+    <t>Ministry of Environment and Water - Executive Environment Agency (ExEA)</t>
+  </si>
+  <si>
+    <t>Australian Antarctic Data Centre</t>
+  </si>
+  <si>
+    <t>Senckenberg Nature Research Society</t>
+  </si>
+  <si>
+    <t>research network</t>
+  </si>
+  <si>
+    <t>Barcode of Life Data System (BOLDSystems)</t>
+  </si>
+  <si>
+    <t>Centre for Biodiversity Genomics (CBG)</t>
+  </si>
+  <si>
+    <t>Marine Conservation Society</t>
+  </si>
+  <si>
+    <t>Ocean Ecology Limited</t>
+  </si>
+  <si>
+    <t>Stanford University - Hopkins Marine Station</t>
+  </si>
+  <si>
+    <t>Swedish Museum of Natural History - Department of Palaeobiology</t>
+  </si>
+  <si>
+    <t>Aquazoo Löbbecke Museum</t>
+  </si>
+  <si>
+    <t>Florida International University</t>
+  </si>
+  <si>
+    <t>Florida Atlantic University - Harbor Branch Oceanographic Institute</t>
+  </si>
+  <si>
+    <t>Northern Ireland Executive - Department of Agriculture, Environment and Rural Affairs (DAERA)</t>
+  </si>
+  <si>
+    <t>India government - Marine Products Export Development Authority (MPEDA)</t>
+  </si>
+  <si>
+    <t>Oceana Europe</t>
+  </si>
+  <si>
+    <t>CRITTERBASE</t>
+  </si>
+  <si>
+    <t>PANGAEA</t>
+  </si>
+  <si>
+    <t>Eco Marine Consultants</t>
+  </si>
+  <si>
+    <t>Add-my-Pet (AmP) </t>
+  </si>
+  <si>
+    <t>BioObs (Base pour l'inventaire des observations subaquatiques)</t>
+  </si>
+  <si>
+    <t>JAMSTEC (Japan Agency for Marine-Earth Science and Technology) - Biological Information System for Marine Life (BISMaL)</t>
+  </si>
+  <si>
+    <t>BlueBRIDGE</t>
+  </si>
+  <si>
+    <t>Données d'Observations pour la Reconnaissance et l'Identification de la faune et la flore Subaquatiques (DORIS)</t>
+  </si>
+  <si>
+    <t>Smithsonian Institution - Smithsonian National Museum of Natural History - Encyclopedia of Life (EOL)</t>
+  </si>
+  <si>
+    <t>Washington State Department of Ecology - Environmental Information Management (EIM) database</t>
+  </si>
+  <si>
+    <t>Foraminifera.eu</t>
+  </si>
+  <si>
+    <t>Bases de données des espèces non-domestiques (BDEND)</t>
+  </si>
+  <si>
+    <t>Natural History Collections of Tyrolean State Museum Ferdinandeum</t>
+  </si>
+  <si>
+    <t>University of Strathclyde - Department of Mathematics and Statistics - Marine Resource Modelling Group</t>
+  </si>
+  <si>
+    <t>Massachusetts Institute of Technology (MIT) - Sea Grant College Program</t>
+  </si>
+  <si>
+    <t>University of Bordeaux - National benthic database</t>
+  </si>
+  <si>
+    <t>Nationalpark Niedersächsisches Wattenmeer</t>
+  </si>
+  <si>
+    <t>Opale Surfcasting</t>
+  </si>
+  <si>
+    <t>Open Tree of Life</t>
+  </si>
+  <si>
+    <t>Alfred Wegener Institute for Polar and Marine Research (AWI) - PAPARA(ZZ)I Annotation tool</t>
+  </si>
+  <si>
+    <t>Central and Northern California Ocean Observing System (CeNCOOS)</t>
+  </si>
+  <si>
+    <t>Sponge Barcoding Project (SBP)</t>
+  </si>
+  <si>
+    <t>Unified Taxonomic Information Service (UTIS)</t>
+  </si>
+  <si>
+    <t>International Atomic Energy Agency (IAEA)</t>
+  </si>
+  <si>
+    <t>S&amp;P Global Inc.</t>
+  </si>
+  <si>
+    <t>International Council on Clean Transportation (ICCT)</t>
+  </si>
+  <si>
+    <t>CRIMARIO</t>
+  </si>
+  <si>
+    <t>EarthScope-Oceans</t>
+  </si>
+  <si>
+    <t>Royal United Services Institute (RUSI)</t>
+  </si>
+  <si>
+    <t>Danish Defence Intelligence Service</t>
+  </si>
+  <si>
+    <t>South African government - Department of Agriculture, Forestry and Fisheries</t>
+  </si>
+  <si>
+    <t>European Maritime Safety Agency</t>
+  </si>
+  <si>
+    <t>Italian Navy - Hydrographic Institute</t>
+  </si>
+  <si>
+    <t>Korean government - Ministry of Oceans and Fisheries - Fisheries Monitoring Center (FMC)</t>
+  </si>
+  <si>
+    <t>Pacific Islands Forum Fisheries Agency</t>
+  </si>
+  <si>
+    <t>UK Space Agency</t>
+  </si>
+  <si>
+    <t>US Department of Veterans Affairs</t>
+  </si>
+  <si>
+    <t>Belgian Offshore Platform</t>
+  </si>
+  <si>
+    <t>IHS Markit</t>
+  </si>
+  <si>
+    <t>PWC</t>
+  </si>
+  <si>
+    <t>OMV Group</t>
+  </si>
+  <si>
+    <t>NKT</t>
+  </si>
+  <si>
+    <t>Nautoshark</t>
+  </si>
+  <si>
+    <t>Seas of Solutions</t>
+  </si>
+  <si>
+    <t>ScanReach</t>
+  </si>
+  <si>
+    <t>Telstra</t>
+  </si>
+  <si>
+    <t>Vickers &amp; Nolan Enterprises, LLC (VNE)</t>
   </si>
 </sst>
 </file>
@@ -8341,11 +8608,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2469"/>
+  <dimension ref="A1:AZ2557"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2529" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2558" sqref="A2558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67299,10 +67566,10 @@
         <v>1972</v>
       </c>
       <c r="D2118" t="s">
-        <v>54</v>
+        <v>279</v>
       </c>
       <c r="E2118" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F2118" t="s">
         <v>55</v>
@@ -77241,7 +77508,1249 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2470" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2470" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2470" t="s">
+        <v>2643</v>
+      </c>
+      <c r="D2470" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2470" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2471" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2471" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2471" t="s">
+        <v>2644</v>
+      </c>
+      <c r="D2471" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2471" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2472" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2472" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2472" t="s">
+        <v>2645</v>
+      </c>
+      <c r="D2472" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2472" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2473" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2473" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2473" t="s">
+        <v>2646</v>
+      </c>
+      <c r="D2473" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2473" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2474" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2474" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2474" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2474" t="s">
+        <v>2647</v>
+      </c>
+      <c r="D2474" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2474" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2475" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2475" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2475" t="s">
+        <v>2648</v>
+      </c>
+      <c r="D2475" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2475" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2476" t="s">
+        <v>617</v>
+      </c>
+      <c r="C2476" t="s">
+        <v>2649</v>
+      </c>
+      <c r="D2476" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2476" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2477" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2477" t="s">
+        <v>2652</v>
+      </c>
+      <c r="C2477" t="s">
+        <v>2650</v>
+      </c>
+      <c r="D2477" t="s">
+        <v>2651</v>
+      </c>
+      <c r="E2477" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2478" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2478" t="s">
+        <v>2653</v>
+      </c>
+      <c r="C2478" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D2478" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2478" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2479" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2479" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C2479" t="s">
+        <v>2654</v>
+      </c>
+      <c r="D2479" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2479" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2480" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2480" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2480" t="s">
+        <v>2655</v>
+      </c>
+      <c r="D2480" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2480" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2481" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2481" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2481" t="s">
+        <v>2656</v>
+      </c>
+      <c r="D2481" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2481" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2482" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2482" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2482" t="s">
+        <v>2657</v>
+      </c>
+      <c r="D2482" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2482" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2483" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2483" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2483" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2483" t="s">
+        <v>2658</v>
+      </c>
+      <c r="D2483" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2483" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2484" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2484" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2484" t="s">
+        <v>2659</v>
+      </c>
+      <c r="D2484" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2484" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2485" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2485" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2485" t="s">
+        <v>2660</v>
+      </c>
+      <c r="D2485" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2485" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2486" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2486" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C2486" t="s">
+        <v>2661</v>
+      </c>
+      <c r="D2486" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2486" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2487" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2487" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2487" t="s">
+        <v>2662</v>
+      </c>
+      <c r="D2487" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2487" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2488" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2488" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2488" t="s">
+        <v>2663</v>
+      </c>
+      <c r="D2488" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2488" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2489" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2489" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2489" t="s">
+        <v>928</v>
+      </c>
+      <c r="D2489" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2489" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2490" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2490" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2490" t="s">
+        <v>2664</v>
+      </c>
+      <c r="D2490" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2490" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2491" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2491" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2491" t="s">
+        <v>2665</v>
+      </c>
+      <c r="D2491" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2491" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2492" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2492" t="s">
+        <v>2576</v>
+      </c>
+      <c r="C2492" t="s">
+        <v>2666</v>
+      </c>
+      <c r="D2492" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2492" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2493" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2493" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C2493" t="s">
+        <v>2667</v>
+      </c>
+      <c r="D2493" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2493" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2494" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2494" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2494" t="s">
+        <v>2668</v>
+      </c>
+      <c r="D2494" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2494" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2495" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2495" t="s">
+        <v>382</v>
+      </c>
+      <c r="C2495" t="s">
+        <v>2669</v>
+      </c>
+      <c r="D2495" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2495" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2496" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2496" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2496" t="s">
+        <v>2670</v>
+      </c>
+      <c r="D2496" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2496" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2497" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2497" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D2497" t="s">
+        <v>2672</v>
+      </c>
+      <c r="E2497" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2498" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2498" t="s">
+        <v>2673</v>
+      </c>
+      <c r="D2498" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2498" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2499" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2499" s="2" t="s">
+        <v>2674</v>
+      </c>
+      <c r="D2499" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2499" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2500" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2500" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2500" t="s">
+        <v>2675</v>
+      </c>
+      <c r="D2500" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2500" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2501" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2501" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2501" t="s">
+        <v>2676</v>
+      </c>
+      <c r="D2501" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2501" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2502" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2502" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2502" t="s">
+        <v>2677</v>
+      </c>
+      <c r="D2502" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2502" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2503" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2503" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C2503" t="s">
+        <v>2678</v>
+      </c>
+      <c r="D2503" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2503" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2504" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2504" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2504" t="s">
+        <v>2679</v>
+      </c>
+      <c r="D2504" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2504" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2505" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2505" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2505" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D2505" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2505" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2506" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2506" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2506" t="s">
+        <v>2681</v>
+      </c>
+      <c r="D2506" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2506" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2507" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2507" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2507" t="s">
+        <v>2682</v>
+      </c>
+      <c r="D2507" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2507" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2508" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2508" t="s">
+        <v>978</v>
+      </c>
+      <c r="C2508" t="s">
+        <v>2683</v>
+      </c>
+      <c r="D2508" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2508" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2509" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2509" t="s">
+        <v>617</v>
+      </c>
+      <c r="C2509" t="s">
+        <v>2684</v>
+      </c>
+      <c r="D2509" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2509" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2510" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2510" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2510" t="s">
+        <v>2685</v>
+      </c>
+      <c r="D2510" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2510" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2511" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2511" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2511" t="s">
+        <v>2686</v>
+      </c>
+      <c r="D2511" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2511" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2512" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2512" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2512" t="s">
+        <v>2687</v>
+      </c>
+      <c r="D2512" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2512" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2513" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2513" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C2513" t="s">
+        <v>2688</v>
+      </c>
+      <c r="D2513" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2513" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2514" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2514" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2514" t="s">
+        <v>2689</v>
+      </c>
+      <c r="D2514" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2514" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2515" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2515" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2515" t="s">
+        <v>2690</v>
+      </c>
+      <c r="D2515" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2515" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2516" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2516" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C2516" t="s">
+        <v>2691</v>
+      </c>
+      <c r="D2516" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2516" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2517" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2517" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2517" t="s">
+        <v>2692</v>
+      </c>
+      <c r="D2517" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2517" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2518" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2518" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2518" t="s">
+        <v>2693</v>
+      </c>
+      <c r="D2518" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2518" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2519" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2519" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2519" t="s">
+        <v>2694</v>
+      </c>
+      <c r="D2519" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2519" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2520" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2520" t="s">
+        <v>617</v>
+      </c>
+      <c r="C2520" t="s">
+        <v>2695</v>
+      </c>
+      <c r="D2520" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2520" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2521" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2521" t="s">
+        <v>617</v>
+      </c>
+      <c r="C2521" t="s">
+        <v>645</v>
+      </c>
+      <c r="D2521" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2521" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2522" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2522" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2522" t="s">
+        <v>2696</v>
+      </c>
+      <c r="D2522" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2522" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2523" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2523" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2523" t="s">
+        <v>2697</v>
+      </c>
+      <c r="D2523" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2523" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2524" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2524" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2524" t="s">
+        <v>2698</v>
+      </c>
+      <c r="D2524" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2524" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2525" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2525" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2525" t="s">
+        <v>2699</v>
+      </c>
+      <c r="D2525" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2525" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2526" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2526" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2526" t="s">
+        <v>2700</v>
+      </c>
+      <c r="D2526" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2526" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2527" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2527" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2527" t="s">
+        <v>2701</v>
+      </c>
+      <c r="D2527" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2527" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2528" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2528" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2528" t="s">
+        <v>2702</v>
+      </c>
+      <c r="D2528" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2528" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2529" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2529" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2529" t="s">
+        <v>2703</v>
+      </c>
+      <c r="D2529" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2529" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2530" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2530" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2530" t="s">
+        <v>2704</v>
+      </c>
+      <c r="D2530" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2530" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2531" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2531" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2531" t="s">
+        <v>2705</v>
+      </c>
+      <c r="D2531" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2531" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2532" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2532" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2532" t="s">
+        <v>2706</v>
+      </c>
+      <c r="D2532" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2532" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2533" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2533" t="s">
+        <v>617</v>
+      </c>
+      <c r="C2533" t="s">
+        <v>2707</v>
+      </c>
+      <c r="D2533" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2533" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2534" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2534" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2534" t="s">
+        <v>2708</v>
+      </c>
+      <c r="D2534" t="s">
+        <v>870</v>
+      </c>
+      <c r="E2534" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2535" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2535" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2535" t="s">
+        <v>2709</v>
+      </c>
+      <c r="D2535" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2535" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2536" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2536" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2536" t="s">
+        <v>2710</v>
+      </c>
+      <c r="D2536" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2536" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2537" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2537" t="s">
+        <v>617</v>
+      </c>
+      <c r="C2537" t="s">
+        <v>2711</v>
+      </c>
+      <c r="D2537" t="s">
+        <v>870</v>
+      </c>
+      <c r="E2537" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2538" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2538" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2538" t="s">
+        <v>2712</v>
+      </c>
+      <c r="D2538" t="s">
+        <v>2672</v>
+      </c>
+      <c r="E2538" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2539" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2539" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2539" t="s">
+        <v>2713</v>
+      </c>
+      <c r="D2539" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2539" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2540" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2540" t="s">
+        <v>577</v>
+      </c>
+      <c r="C2540" t="s">
+        <v>2714</v>
+      </c>
+      <c r="D2540" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2540" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2541" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2541" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C2541" t="s">
+        <v>2715</v>
+      </c>
+      <c r="D2541" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2541" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2542" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2542" t="s">
+        <v>617</v>
+      </c>
+      <c r="C2542" t="s">
+        <v>2716</v>
+      </c>
+      <c r="D2542" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2542" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2543" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2543" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2543" t="s">
+        <v>2717</v>
+      </c>
+      <c r="D2543" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2543" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2544" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2544" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C2544" t="s">
+        <v>2718</v>
+      </c>
+      <c r="D2544" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2544" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2545" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2545" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2545" t="s">
+        <v>2719</v>
+      </c>
+      <c r="D2545" t="s">
+        <v>870</v>
+      </c>
+      <c r="E2545" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2546" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2546" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2546" t="s">
+        <v>2720</v>
+      </c>
+      <c r="D2546" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2546" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2547" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2547" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2547" t="s">
+        <v>2721</v>
+      </c>
+      <c r="D2547" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2547" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2548" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2548" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2548" t="s">
+        <v>2722</v>
+      </c>
+      <c r="D2548" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2548" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2549" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2549" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2549" t="s">
+        <v>2723</v>
+      </c>
+      <c r="D2549" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2549" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2550" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2550" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2550" t="s">
+        <v>2724</v>
+      </c>
+      <c r="D2550" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2550" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2551" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2551" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2551" t="s">
+        <v>2725</v>
+      </c>
+      <c r="D2551" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2551" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2552" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2552" t="s">
+        <v>577</v>
+      </c>
+      <c r="C2552" t="s">
+        <v>2726</v>
+      </c>
+      <c r="D2552" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2552" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2553" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2553" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2553" t="s">
+        <v>2727</v>
+      </c>
+      <c r="D2553" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2553" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2554" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2554" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C2554" t="s">
+        <v>2728</v>
+      </c>
+      <c r="D2554" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2554" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2555" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2555" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C2555" t="s">
+        <v>2729</v>
+      </c>
+      <c r="D2555" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2555" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2556" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2556" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2556" t="s">
+        <v>2730</v>
+      </c>
+      <c r="D2556" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2556" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2557" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2557" t="s">
+        <v>2731</v>
+      </c>
+      <c r="D2557" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2557" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:AZ2527" xr:uid="{0BDF6F9C-D91E-49CF-9ECB-F3D5EC4564BE}"/>
   <sortState ref="A2:AZ2470">
     <sortCondition ref="A2:A2470"/>
     <sortCondition ref="C2:C2470"/>

</xml_diff>

<commit_message>
Adding manual standardization of registered users
</commit_message>
<xml_diff>
--- a/reference_data/Affiliations_info.xlsx
+++ b/reference_data/Affiliations_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurian.van.maldeghe\Documents\user-analysis\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CFDDA4-1EB8-4F03-BEB7-3F853A90FA91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F44183-1AF9-4D91-9BCC-01A7AFF74A23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122B1F59-D82E-4685-8764-6F42BE50E31B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Unique_Affiliations" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unique_Affiliations!$A$1:$AZ$2527</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unique_Affiliations!$A$1:$AZ$2592</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12834" uniqueCount="2732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13044" uniqueCount="2784">
   <si>
     <t>Country_stand</t>
   </si>
@@ -7971,9 +7971,6 @@
     <t>Australian National University - Research school of Earth Sciences</t>
   </si>
   <si>
-    <t>De Noordzee</t>
-  </si>
-  <si>
     <t>Natuur En Milieu</t>
   </si>
   <si>
@@ -8224,6 +8221,165 @@
   </si>
   <si>
     <t>Vickers &amp; Nolan Enterprises, LLC (VNE)</t>
+  </si>
+  <si>
+    <t>Marine Data Archive (MDA)</t>
+  </si>
+  <si>
+    <t>Aarhus University - Department of Ecoscience</t>
+  </si>
+  <si>
+    <t>Agnes Scott College</t>
+  </si>
+  <si>
+    <t>Benthic Solutions Limited</t>
+  </si>
+  <si>
+    <t>Biologic Environmental</t>
+  </si>
+  <si>
+    <t>Black &amp; Veatch</t>
+  </si>
+  <si>
+    <t>Carleton University</t>
+  </si>
+  <si>
+    <t>Cefas Technology Ltd</t>
+  </si>
+  <si>
+    <t>CGIAR</t>
+  </si>
+  <si>
+    <t>City of Antwerp</t>
+  </si>
+  <si>
+    <t>De Rijke Noordzee</t>
+  </si>
+  <si>
+    <t>Australian Government - Department of Agriculture, Water and the Environment</t>
+  </si>
+  <si>
+    <t>EcoAnalysts Inc.</t>
+  </si>
+  <si>
+    <t>Exa Data &amp; Mapping Services</t>
+  </si>
+  <si>
+    <t>France Energie Marines</t>
+  </si>
+  <si>
+    <t>Geoinformatics Solutions</t>
+  </si>
+  <si>
+    <t>Government of Jersey</t>
+  </si>
+  <si>
+    <t>Harokopio University</t>
+  </si>
+  <si>
+    <t>Helmholtz Zentrum Hereon</t>
+  </si>
+  <si>
+    <t>Herzog Anton Ulrich Museum</t>
+  </si>
+  <si>
+    <t>HiDef Environmental Consultancy</t>
+  </si>
+  <si>
+    <t>Início Escola Superior Náutica Infante D. Henrique</t>
+  </si>
+  <si>
+    <t>Institute of Agrifood Research and Technology (IRTA)</t>
+  </si>
+  <si>
+    <t>Instituut Biologie Leiden (IBL)</t>
+  </si>
+  <si>
+    <t>Israel Oceanographic &amp; Limnological Research</t>
+  </si>
+  <si>
+    <t>Isreal</t>
+  </si>
+  <si>
+    <t>Landesforschungsanstalt für Landwirtschaft und Fischerei</t>
+  </si>
+  <si>
+    <t>Louisiana State University</t>
+  </si>
+  <si>
+    <t>Marine Ecology and Telemetry Research</t>
+  </si>
+  <si>
+    <t>Météo-France</t>
+  </si>
+  <si>
+    <t>Morant Wright Japan Income Trust Ltd Fund</t>
+  </si>
+  <si>
+    <t>National Centre For Scientific Research - Institute of Informatics and Telecommunications</t>
+  </si>
+  <si>
+    <t>Natural Resources Wales</t>
+  </si>
+  <si>
+    <t>Norwegian Research Centre</t>
+  </si>
+  <si>
+    <t>Parc naturel Hautes Fagnes-Eifel</t>
+  </si>
+  <si>
+    <t>Pelagia Nature &amp; Environment AB</t>
+  </si>
+  <si>
+    <t>personal</t>
+  </si>
+  <si>
+    <t>Polytechnic University of Turin </t>
+  </si>
+  <si>
+    <t>Polytechnic University of Valencia (UPV) - Department of Animal Science</t>
+  </si>
+  <si>
+    <t>Profish Technology</t>
+  </si>
+  <si>
+    <t>RUCO Limited</t>
+  </si>
+  <si>
+    <t>Star-Oddi</t>
+  </si>
+  <si>
+    <t>State University of New York at Fredonia</t>
+  </si>
+  <si>
+    <t>Scottish Government</t>
+  </si>
+  <si>
+    <t>TotalEnergies</t>
+  </si>
+  <si>
+    <t>Tractebel ENGIE</t>
+  </si>
+  <si>
+    <t>UK government - Hydrographics Office</t>
+  </si>
+  <si>
+    <t>University of Montreal</t>
+  </si>
+  <si>
+    <t>University of Silesia</t>
+  </si>
+  <si>
+    <t>University of Southern Denmark - Department of Biology</t>
+  </si>
+  <si>
+    <t>University of Tuscia</t>
+  </si>
+  <si>
+    <t>University of Exeter</t>
+  </si>
+  <si>
+    <t>Vinga Konstruktion AB</t>
   </si>
 </sst>
 </file>
@@ -8286,7 +8442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8294,6 +8450,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8608,11 +8766,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FC6395-9F37-404F-ADBA-7A4B276FFF38}">
-  <dimension ref="A1:AZ2557"/>
+  <dimension ref="A1:AZ2609"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2529" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2558" sqref="A2558"/>
+      <pane ySplit="1" topLeftCell="A2595" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2610" sqref="D2610"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -77571,8 +77729,8 @@
       <c r="B2474" t="s">
         <v>55</v>
       </c>
-      <c r="C2474" t="s">
-        <v>2647</v>
+      <c r="C2474" s="5" t="s">
+        <v>2741</v>
       </c>
       <c r="D2474" t="s">
         <v>279</v>
@@ -77589,7 +77747,7 @@
         <v>55</v>
       </c>
       <c r="C2475" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="D2475" t="s">
         <v>279</v>
@@ -77603,7 +77761,7 @@
         <v>617</v>
       </c>
       <c r="C2476" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D2476" t="s">
         <v>88</v>
@@ -77614,13 +77772,13 @@
     </row>
     <row r="2477" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2477" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="C2477" t="s">
+        <v>2767</v>
+      </c>
+      <c r="D2477" t="s">
         <v>2650</v>
-      </c>
-      <c r="D2477" t="s">
-        <v>2651</v>
       </c>
       <c r="E2477" t="s">
         <v>172</v>
@@ -77628,44 +77786,44 @@
     </row>
     <row r="2478" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2478" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="C2478" t="s">
-        <v>1433</v>
+        <v>2649</v>
       </c>
       <c r="D2478" t="s">
-        <v>201</v>
+        <v>2650</v>
       </c>
       <c r="E2478" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2479" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2479" t="s">
-        <v>1315</v>
+        <v>2652</v>
       </c>
       <c r="C2479" t="s">
-        <v>2654</v>
+        <v>1433</v>
       </c>
       <c r="D2479" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="E2479" t="s">
-        <v>172</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2480" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2480" t="s">
-        <v>868</v>
+        <v>1315</v>
       </c>
       <c r="C2480" t="s">
-        <v>2655</v>
+        <v>2653</v>
       </c>
       <c r="D2480" t="s">
-        <v>199</v>
+        <v>279</v>
       </c>
       <c r="E2480" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2481" spans="1:5" x14ac:dyDescent="0.25">
@@ -77673,7 +77831,7 @@
         <v>868</v>
       </c>
       <c r="C2481" t="s">
-        <v>2656</v>
+        <v>2654</v>
       </c>
       <c r="D2481" t="s">
         <v>199</v>
@@ -77684,27 +77842,24 @@
     </row>
     <row r="2482" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2482" t="s">
-        <v>326</v>
+        <v>868</v>
       </c>
       <c r="C2482" t="s">
-        <v>2657</v>
+        <v>2655</v>
       </c>
       <c r="D2482" t="s">
-        <v>60</v>
+        <v>199</v>
       </c>
       <c r="E2482" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2483" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2483" t="s">
-        <v>194</v>
-      </c>
-      <c r="B2483" t="s">
-        <v>55</v>
+        <v>326</v>
       </c>
       <c r="C2483" t="s">
-        <v>2658</v>
+        <v>2656</v>
       </c>
       <c r="D2483" t="s">
         <v>60</v>
@@ -77717,36 +77872,39 @@
       <c r="A2484" t="s">
         <v>194</v>
       </c>
+      <c r="B2484" t="s">
+        <v>55</v>
+      </c>
       <c r="C2484" t="s">
-        <v>2659</v>
+        <v>2657</v>
       </c>
       <c r="D2484" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="E2484" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2485" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2485" t="s">
-        <v>1984</v>
+        <v>194</v>
       </c>
       <c r="C2485" t="s">
-        <v>2660</v>
+        <v>2658</v>
       </c>
       <c r="D2485" t="s">
-        <v>281</v>
+        <v>88</v>
       </c>
       <c r="E2485" t="s">
-        <v>172</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2486" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2486" t="s">
-        <v>1315</v>
+        <v>1984</v>
       </c>
       <c r="C2486" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="D2486" t="s">
         <v>281</v>
@@ -77757,10 +77915,10 @@
     </row>
     <row r="2487" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2487" t="s">
-        <v>1984</v>
+        <v>1315</v>
       </c>
       <c r="C2487" t="s">
-        <v>2662</v>
+        <v>2660</v>
       </c>
       <c r="D2487" t="s">
         <v>281</v>
@@ -77771,16 +77929,16 @@
     </row>
     <row r="2488" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2488" t="s">
-        <v>868</v>
+        <v>1984</v>
       </c>
       <c r="C2488" t="s">
-        <v>2663</v>
+        <v>2661</v>
       </c>
       <c r="D2488" t="s">
-        <v>199</v>
+        <v>281</v>
       </c>
       <c r="E2488" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2489" spans="1:5" x14ac:dyDescent="0.25">
@@ -77788,7 +77946,7 @@
         <v>868</v>
       </c>
       <c r="C2489" t="s">
-        <v>928</v>
+        <v>2662</v>
       </c>
       <c r="D2489" t="s">
         <v>199</v>
@@ -77802,7 +77960,7 @@
         <v>868</v>
       </c>
       <c r="C2490" t="s">
-        <v>2664</v>
+        <v>928</v>
       </c>
       <c r="D2490" t="s">
         <v>199</v>
@@ -77816,38 +77974,38 @@
         <v>868</v>
       </c>
       <c r="C2491" t="s">
-        <v>2665</v>
+        <v>2663</v>
       </c>
       <c r="D2491" t="s">
-        <v>281</v>
+        <v>199</v>
       </c>
       <c r="E2491" t="s">
-        <v>172</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2492" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2492" t="s">
-        <v>2576</v>
+        <v>868</v>
       </c>
       <c r="C2492" t="s">
-        <v>2666</v>
+        <v>2664</v>
       </c>
       <c r="D2492" t="s">
-        <v>54</v>
+        <v>281</v>
       </c>
       <c r="E2492" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2493" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2493" t="s">
-        <v>1023</v>
+        <v>2576</v>
       </c>
       <c r="C2493" t="s">
-        <v>2667</v>
+        <v>2665</v>
       </c>
       <c r="D2493" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="E2493" t="s">
         <v>5</v>
@@ -77855,55 +78013,55 @@
     </row>
     <row r="2494" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2494" t="s">
-        <v>473</v>
+        <v>1023</v>
       </c>
       <c r="C2494" t="s">
-        <v>2668</v>
+        <v>2666</v>
       </c>
       <c r="D2494" t="s">
-        <v>201</v>
+        <v>88</v>
       </c>
       <c r="E2494" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2495" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2495" t="s">
-        <v>382</v>
+        <v>473</v>
       </c>
       <c r="C2495" t="s">
-        <v>2669</v>
+        <v>2667</v>
       </c>
       <c r="D2495" t="s">
-        <v>60</v>
+        <v>201</v>
       </c>
       <c r="E2495" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2496" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2496" t="s">
-        <v>85</v>
+        <v>382</v>
       </c>
       <c r="C2496" t="s">
-        <v>2670</v>
+        <v>2668</v>
       </c>
       <c r="D2496" t="s">
-        <v>199</v>
+        <v>60</v>
       </c>
       <c r="E2496" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2497" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2497" t="s">
-        <v>755</v>
+        <v>85</v>
       </c>
       <c r="C2497" t="s">
-        <v>2671</v>
+        <v>2669</v>
       </c>
       <c r="D2497" t="s">
-        <v>2672</v>
+        <v>199</v>
       </c>
       <c r="E2497" t="s">
         <v>5</v>
@@ -77911,13 +78069,13 @@
     </row>
     <row r="2498" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2498" t="s">
-        <v>868</v>
+        <v>755</v>
       </c>
       <c r="C2498" t="s">
-        <v>2673</v>
+        <v>2670</v>
       </c>
       <c r="D2498" t="s">
-        <v>199</v>
+        <v>2671</v>
       </c>
       <c r="E2498" t="s">
         <v>5</v>
@@ -77925,13 +78083,13 @@
     </row>
     <row r="2499" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2499" t="s">
-        <v>384</v>
-      </c>
-      <c r="C2499" s="2" t="s">
-        <v>2674</v>
+        <v>868</v>
+      </c>
+      <c r="C2499" t="s">
+        <v>2672</v>
       </c>
       <c r="D2499" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="E2499" t="s">
         <v>5</v>
@@ -77939,16 +78097,16 @@
     </row>
     <row r="2500" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2500" t="s">
-        <v>1841</v>
-      </c>
-      <c r="C2500" t="s">
-        <v>2675</v>
+        <v>384</v>
+      </c>
+      <c r="C2500" s="2" t="s">
+        <v>2673</v>
       </c>
       <c r="D2500" t="s">
-        <v>279</v>
+        <v>88</v>
       </c>
       <c r="E2500" t="s">
-        <v>172</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2501" spans="1:5" x14ac:dyDescent="0.25">
@@ -77956,38 +78114,38 @@
         <v>1841</v>
       </c>
       <c r="C2501" t="s">
-        <v>2676</v>
+        <v>2674</v>
       </c>
       <c r="D2501" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="E2501" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2502" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2502" t="s">
-        <v>1984</v>
+        <v>1841</v>
       </c>
       <c r="C2502" t="s">
-        <v>2677</v>
+        <v>2675</v>
       </c>
       <c r="D2502" t="s">
-        <v>88</v>
+        <v>208</v>
       </c>
       <c r="E2502" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2503" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2503" t="s">
-        <v>1737</v>
+        <v>1984</v>
       </c>
       <c r="C2503" t="s">
-        <v>2678</v>
+        <v>2676</v>
       </c>
       <c r="D2503" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="E2503" t="s">
         <v>5</v>
@@ -77995,10 +78153,10 @@
     </row>
     <row r="2504" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2504" t="s">
-        <v>755</v>
+        <v>1737</v>
       </c>
       <c r="C2504" t="s">
-        <v>2679</v>
+        <v>2677</v>
       </c>
       <c r="D2504" t="s">
         <v>58</v>
@@ -78009,13 +78167,13 @@
     </row>
     <row r="2505" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2505" t="s">
-        <v>1984</v>
+        <v>755</v>
       </c>
       <c r="C2505" t="s">
-        <v>2680</v>
+        <v>2678</v>
       </c>
       <c r="D2505" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E2505" t="s">
         <v>5</v>
@@ -78026,10 +78184,10 @@
         <v>1984</v>
       </c>
       <c r="C2506" t="s">
-        <v>2681</v>
+        <v>2679</v>
       </c>
       <c r="D2506" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="E2506" t="s">
         <v>5</v>
@@ -78037,24 +78195,24 @@
     </row>
     <row r="2507" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2507" t="s">
-        <v>1841</v>
+        <v>1984</v>
       </c>
       <c r="C2507" t="s">
-        <v>2682</v>
+        <v>2680</v>
       </c>
       <c r="D2507" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="E2507" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2508" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2508" t="s">
-        <v>978</v>
+        <v>1841</v>
       </c>
       <c r="C2508" t="s">
-        <v>2683</v>
+        <v>2681</v>
       </c>
       <c r="D2508" t="s">
         <v>60</v>
@@ -78065,30 +78223,30 @@
     </row>
     <row r="2509" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2509" t="s">
-        <v>617</v>
+        <v>978</v>
       </c>
       <c r="C2509" t="s">
-        <v>2684</v>
+        <v>2682</v>
       </c>
       <c r="D2509" t="s">
-        <v>279</v>
+        <v>60</v>
       </c>
       <c r="E2509" t="s">
-        <v>172</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2510" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2510" t="s">
-        <v>755</v>
+        <v>617</v>
       </c>
       <c r="C2510" t="s">
-        <v>2685</v>
+        <v>2683</v>
       </c>
       <c r="D2510" t="s">
-        <v>199</v>
+        <v>279</v>
       </c>
       <c r="E2510" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2511" spans="1:5" x14ac:dyDescent="0.25">
@@ -78096,7 +78254,7 @@
         <v>755</v>
       </c>
       <c r="C2511" t="s">
-        <v>2686</v>
+        <v>2684</v>
       </c>
       <c r="D2511" t="s">
         <v>199</v>
@@ -78107,38 +78265,38 @@
     </row>
     <row r="2512" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2512" t="s">
-        <v>1841</v>
+        <v>755</v>
       </c>
       <c r="C2512" t="s">
-        <v>2687</v>
+        <v>2685</v>
       </c>
       <c r="D2512" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="E2512" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2513" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2513" t="s">
-        <v>1315</v>
+        <v>1841</v>
       </c>
       <c r="C2513" t="s">
-        <v>2688</v>
+        <v>2686</v>
       </c>
       <c r="D2513" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="E2513" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2514" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2514" t="s">
-        <v>659</v>
+        <v>1315</v>
       </c>
       <c r="C2514" t="s">
-        <v>2689</v>
+        <v>2687</v>
       </c>
       <c r="D2514" t="s">
         <v>199</v>
@@ -78149,10 +78307,10 @@
     </row>
     <row r="2515" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2515" t="s">
-        <v>1185</v>
+        <v>659</v>
       </c>
       <c r="C2515" t="s">
-        <v>2690</v>
+        <v>2688</v>
       </c>
       <c r="D2515" t="s">
         <v>199</v>
@@ -78163,38 +78321,38 @@
     </row>
     <row r="2516" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2516" t="s">
-        <v>1353</v>
+        <v>1185</v>
       </c>
       <c r="C2516" t="s">
-        <v>2691</v>
+        <v>2689</v>
       </c>
       <c r="D2516" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="E2516" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2517" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2517" t="s">
-        <v>659</v>
+        <v>1353</v>
       </c>
       <c r="C2517" t="s">
-        <v>2692</v>
+        <v>2690</v>
       </c>
       <c r="D2517" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="E2517" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2518" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2518" t="s">
-        <v>1984</v>
+        <v>659</v>
       </c>
       <c r="C2518" t="s">
-        <v>2693</v>
+        <v>2691</v>
       </c>
       <c r="D2518" t="s">
         <v>199</v>
@@ -78208,7 +78366,7 @@
         <v>1984</v>
       </c>
       <c r="C2519" t="s">
-        <v>2694</v>
+        <v>2692</v>
       </c>
       <c r="D2519" t="s">
         <v>199</v>
@@ -78219,13 +78377,13 @@
     </row>
     <row r="2520" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2520" t="s">
-        <v>617</v>
+        <v>1984</v>
       </c>
       <c r="C2520" t="s">
-        <v>2695</v>
+        <v>2693</v>
       </c>
       <c r="D2520" t="s">
-        <v>281</v>
+        <v>199</v>
       </c>
       <c r="E2520" t="s">
         <v>5</v>
@@ -78236,10 +78394,10 @@
         <v>617</v>
       </c>
       <c r="C2521" t="s">
-        <v>645</v>
+        <v>2694</v>
       </c>
       <c r="D2521" t="s">
-        <v>199</v>
+        <v>281</v>
       </c>
       <c r="E2521" t="s">
         <v>5</v>
@@ -78247,10 +78405,10 @@
     </row>
     <row r="2522" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2522" t="s">
-        <v>659</v>
+        <v>617</v>
       </c>
       <c r="C2522" t="s">
-        <v>2696</v>
+        <v>645</v>
       </c>
       <c r="D2522" t="s">
         <v>199</v>
@@ -78261,13 +78419,13 @@
     </row>
     <row r="2523" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2523" t="s">
-        <v>168</v>
+        <v>659</v>
       </c>
       <c r="C2523" t="s">
-        <v>2697</v>
+        <v>2695</v>
       </c>
       <c r="D2523" t="s">
-        <v>58</v>
+        <v>199</v>
       </c>
       <c r="E2523" t="s">
         <v>5</v>
@@ -78275,13 +78433,13 @@
     </row>
     <row r="2524" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2524" t="s">
-        <v>1841</v>
+        <v>168</v>
       </c>
       <c r="C2524" t="s">
-        <v>2698</v>
+        <v>2696</v>
       </c>
       <c r="D2524" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E2524" t="s">
         <v>5</v>
@@ -78289,13 +78447,13 @@
     </row>
     <row r="2525" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2525" t="s">
-        <v>1984</v>
+        <v>1841</v>
       </c>
       <c r="C2525" t="s">
-        <v>2699</v>
+        <v>2697</v>
       </c>
       <c r="D2525" t="s">
-        <v>199</v>
+        <v>54</v>
       </c>
       <c r="E2525" t="s">
         <v>5</v>
@@ -78303,10 +78461,10 @@
     </row>
     <row r="2526" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2526" t="s">
-        <v>659</v>
+        <v>1984</v>
       </c>
       <c r="C2526" t="s">
-        <v>2700</v>
+        <v>2698</v>
       </c>
       <c r="D2526" t="s">
         <v>199</v>
@@ -78317,30 +78475,30 @@
     </row>
     <row r="2527" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2527" t="s">
-        <v>755</v>
+        <v>659</v>
       </c>
       <c r="C2527" t="s">
-        <v>2701</v>
+        <v>2699</v>
       </c>
       <c r="D2527" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="E2527" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2528" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2528" t="s">
-        <v>868</v>
+        <v>755</v>
       </c>
       <c r="C2528" t="s">
-        <v>2702</v>
+        <v>2700</v>
       </c>
       <c r="D2528" t="s">
-        <v>281</v>
+        <v>175</v>
       </c>
       <c r="E2528" t="s">
-        <v>172</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2529" spans="1:5" x14ac:dyDescent="0.25">
@@ -78348,21 +78506,21 @@
         <v>868</v>
       </c>
       <c r="C2529" t="s">
-        <v>2703</v>
+        <v>2701</v>
       </c>
       <c r="D2529" t="s">
-        <v>199</v>
+        <v>281</v>
       </c>
       <c r="E2529" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2530" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2530" t="s">
-        <v>755</v>
+        <v>868</v>
       </c>
       <c r="C2530" t="s">
-        <v>2704</v>
+        <v>2702</v>
       </c>
       <c r="D2530" t="s">
         <v>199</v>
@@ -78373,10 +78531,10 @@
     </row>
     <row r="2531" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2531" t="s">
-        <v>1984</v>
+        <v>755</v>
       </c>
       <c r="C2531" t="s">
-        <v>2705</v>
+        <v>2703</v>
       </c>
       <c r="D2531" t="s">
         <v>199</v>
@@ -78387,10 +78545,10 @@
     </row>
     <row r="2532" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2532" t="s">
-        <v>868</v>
+        <v>1984</v>
       </c>
       <c r="C2532" t="s">
-        <v>2706</v>
+        <v>2704</v>
       </c>
       <c r="D2532" t="s">
         <v>199</v>
@@ -78401,10 +78559,10 @@
     </row>
     <row r="2533" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2533" t="s">
-        <v>617</v>
+        <v>868</v>
       </c>
       <c r="C2533" t="s">
-        <v>2707</v>
+        <v>2705</v>
       </c>
       <c r="D2533" t="s">
         <v>199</v>
@@ -78415,27 +78573,27 @@
     </row>
     <row r="2534" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2534" t="s">
-        <v>868</v>
+        <v>617</v>
       </c>
       <c r="C2534" t="s">
-        <v>2708</v>
+        <v>2706</v>
       </c>
       <c r="D2534" t="s">
-        <v>870</v>
+        <v>199</v>
       </c>
       <c r="E2534" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2535" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2535" t="s">
-        <v>1984</v>
+        <v>868</v>
       </c>
       <c r="C2535" t="s">
-        <v>2709</v>
+        <v>2707</v>
       </c>
       <c r="D2535" t="s">
-        <v>201</v>
+        <v>870</v>
       </c>
       <c r="E2535" t="s">
         <v>7</v>
@@ -78443,66 +78601,66 @@
     </row>
     <row r="2536" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2536" t="s">
-        <v>868</v>
+        <v>1984</v>
       </c>
       <c r="C2536" t="s">
-        <v>2710</v>
+        <v>2708</v>
       </c>
       <c r="D2536" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="E2536" t="s">
-        <v>172</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2537" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2537" t="s">
-        <v>617</v>
+        <v>868</v>
       </c>
       <c r="C2537" t="s">
-        <v>2711</v>
+        <v>2709</v>
       </c>
       <c r="D2537" t="s">
-        <v>870</v>
+        <v>279</v>
       </c>
       <c r="E2537" t="s">
-        <v>7</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2538" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2538" t="s">
-        <v>868</v>
+        <v>617</v>
       </c>
       <c r="C2538" t="s">
-        <v>2712</v>
+        <v>2710</v>
       </c>
       <c r="D2538" t="s">
-        <v>2672</v>
+        <v>870</v>
       </c>
       <c r="E2538" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2539" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2539" t="s">
-        <v>1841</v>
+        <v>868</v>
       </c>
       <c r="C2539" t="s">
-        <v>2713</v>
+        <v>2711</v>
       </c>
       <c r="D2539" t="s">
-        <v>60</v>
+        <v>2671</v>
       </c>
       <c r="E2539" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2540" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2540" t="s">
-        <v>577</v>
+        <v>1841</v>
       </c>
       <c r="C2540" t="s">
-        <v>2714</v>
+        <v>2712</v>
       </c>
       <c r="D2540" t="s">
         <v>60</v>
@@ -78513,10 +78671,10 @@
     </row>
     <row r="2541" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2541" t="s">
-        <v>1570</v>
+        <v>577</v>
       </c>
       <c r="C2541" t="s">
-        <v>2715</v>
+        <v>2713</v>
       </c>
       <c r="D2541" t="s">
         <v>60</v>
@@ -78527,10 +78685,10 @@
     </row>
     <row r="2542" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2542" t="s">
-        <v>617</v>
+        <v>1570</v>
       </c>
       <c r="C2542" t="s">
-        <v>2716</v>
+        <v>2714</v>
       </c>
       <c r="D2542" t="s">
         <v>60</v>
@@ -78541,10 +78699,10 @@
     </row>
     <row r="2543" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2543" t="s">
-        <v>1093</v>
+        <v>617</v>
       </c>
       <c r="C2543" t="s">
-        <v>2717</v>
+        <v>2715</v>
       </c>
       <c r="D2543" t="s">
         <v>60</v>
@@ -78555,10 +78713,10 @@
     </row>
     <row r="2544" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2544" t="s">
-        <v>1608</v>
+        <v>1093</v>
       </c>
       <c r="C2544" t="s">
-        <v>2718</v>
+        <v>2716</v>
       </c>
       <c r="D2544" t="s">
         <v>60</v>
@@ -78569,13 +78727,13 @@
     </row>
     <row r="2545" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2545" t="s">
-        <v>868</v>
+        <v>1608</v>
       </c>
       <c r="C2545" t="s">
-        <v>2719</v>
+        <v>2717</v>
       </c>
       <c r="D2545" t="s">
-        <v>870</v>
+        <v>60</v>
       </c>
       <c r="E2545" t="s">
         <v>7</v>
@@ -78583,58 +78741,58 @@
     </row>
     <row r="2546" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2546" t="s">
-        <v>1841</v>
+        <v>868</v>
       </c>
       <c r="C2546" t="s">
-        <v>2720</v>
+        <v>2718</v>
       </c>
       <c r="D2546" t="s">
-        <v>88</v>
+        <v>870</v>
       </c>
       <c r="E2546" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2547" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2547" t="s">
-        <v>1984</v>
+        <v>1841</v>
       </c>
       <c r="C2547" t="s">
-        <v>2721</v>
+        <v>2719</v>
       </c>
       <c r="D2547" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="E2547" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2548" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2548" t="s">
-        <v>194</v>
+        <v>1984</v>
       </c>
       <c r="C2548" t="s">
-        <v>2722</v>
+        <v>2720</v>
       </c>
       <c r="D2548" t="s">
-        <v>279</v>
+        <v>60</v>
       </c>
       <c r="E2548" t="s">
-        <v>172</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2549" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2549" t="s">
-        <v>1841</v>
+        <v>194</v>
       </c>
       <c r="C2549" t="s">
-        <v>2723</v>
+        <v>2721</v>
       </c>
       <c r="D2549" t="s">
-        <v>201</v>
+        <v>279</v>
       </c>
       <c r="E2549" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2550" spans="1:5" x14ac:dyDescent="0.25">
@@ -78642,7 +78800,7 @@
         <v>1841</v>
       </c>
       <c r="C2550" t="s">
-        <v>2724</v>
+        <v>2722</v>
       </c>
       <c r="D2550" t="s">
         <v>201</v>
@@ -78653,10 +78811,10 @@
     </row>
     <row r="2551" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2551" t="s">
-        <v>168</v>
+        <v>1841</v>
       </c>
       <c r="C2551" t="s">
-        <v>2725</v>
+        <v>2723</v>
       </c>
       <c r="D2551" t="s">
         <v>201</v>
@@ -78667,10 +78825,10 @@
     </row>
     <row r="2552" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2552" t="s">
-        <v>577</v>
+        <v>168</v>
       </c>
       <c r="C2552" t="s">
-        <v>2726</v>
+        <v>2724</v>
       </c>
       <c r="D2552" t="s">
         <v>201</v>
@@ -78681,10 +78839,10 @@
     </row>
     <row r="2553" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2553" t="s">
-        <v>1841</v>
+        <v>577</v>
       </c>
       <c r="C2553" t="s">
-        <v>2727</v>
+        <v>2725</v>
       </c>
       <c r="D2553" t="s">
         <v>201</v>
@@ -78695,10 +78853,10 @@
     </row>
     <row r="2554" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2554" t="s">
-        <v>1315</v>
+        <v>1841</v>
       </c>
       <c r="C2554" t="s">
-        <v>2728</v>
+        <v>2726</v>
       </c>
       <c r="D2554" t="s">
         <v>201</v>
@@ -78709,10 +78867,10 @@
     </row>
     <row r="2555" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2555" t="s">
-        <v>1378</v>
+        <v>1315</v>
       </c>
       <c r="C2555" t="s">
-        <v>2729</v>
+        <v>2727</v>
       </c>
       <c r="D2555" t="s">
         <v>201</v>
@@ -78723,10 +78881,10 @@
     </row>
     <row r="2556" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2556" t="s">
-        <v>85</v>
+        <v>1378</v>
       </c>
       <c r="C2556" t="s">
-        <v>2730</v>
+        <v>2728</v>
       </c>
       <c r="D2556" t="s">
         <v>201</v>
@@ -78737,10 +78895,10 @@
     </row>
     <row r="2557" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2557" t="s">
-        <v>1984</v>
+        <v>85</v>
       </c>
       <c r="C2557" t="s">
-        <v>2731</v>
+        <v>2729</v>
       </c>
       <c r="D2557" t="s">
         <v>201</v>
@@ -78749,8 +78907,742 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2558" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2558" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2558" t="s">
+        <v>2730</v>
+      </c>
+      <c r="D2558" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2558" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2559" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2559" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2559" s="2" t="s">
+        <v>2731</v>
+      </c>
+      <c r="D2559" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2559" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2560" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2560" t="s">
+        <v>577</v>
+      </c>
+      <c r="C2560" t="s">
+        <v>2732</v>
+      </c>
+      <c r="D2560" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2560" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2561" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2561" t="s">
+        <v>2733</v>
+      </c>
+      <c r="D2561" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2561" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2562" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2562" t="s">
+        <v>2734</v>
+      </c>
+      <c r="D2562" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2562" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2563" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2563" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2563" t="s">
+        <v>2735</v>
+      </c>
+      <c r="D2563" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2563" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2564" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2564" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2564" t="s">
+        <v>2736</v>
+      </c>
+      <c r="D2564" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2564" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2565" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2565" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2565" t="s">
+        <v>2737</v>
+      </c>
+      <c r="D2565" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2565" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2566" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2566" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2566" t="s">
+        <v>2738</v>
+      </c>
+      <c r="D2566" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2566" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2567" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2567" s="5" t="s">
+        <v>2739</v>
+      </c>
+      <c r="D2567" t="s">
+        <v>270</v>
+      </c>
+      <c r="E2567" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2568" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2568" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2568" s="6" t="s">
+        <v>2740</v>
+      </c>
+      <c r="D2568" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2568" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2569" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2569" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2569" s="5" t="s">
+        <v>2742</v>
+      </c>
+      <c r="D2569" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2569" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2570" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2570" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2570" t="s">
+        <v>2743</v>
+      </c>
+      <c r="D2570" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2570" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2571" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2571" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2571" t="s">
+        <v>2744</v>
+      </c>
+      <c r="D2571" t="s">
+        <v>270</v>
+      </c>
+      <c r="E2571" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2572" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2572" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2572" s="5" t="s">
+        <v>1868</v>
+      </c>
+      <c r="D2572" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2572" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2573" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2573" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2573" s="5" t="s">
+        <v>2745</v>
+      </c>
+      <c r="D2573" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2573" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2574" t="s">
+        <v>933</v>
+      </c>
+      <c r="C2574" s="5" t="s">
+        <v>2746</v>
+      </c>
+      <c r="D2574" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2574" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2575" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2575" t="s">
+        <v>2747</v>
+      </c>
+      <c r="D2575" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2575" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2576" t="s">
+        <v>933</v>
+      </c>
+      <c r="C2576" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D2576" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2576" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2577" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2577" t="s">
+        <v>2749</v>
+      </c>
+      <c r="D2577" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2577" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2578" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2578" t="s">
+        <v>2750</v>
+      </c>
+      <c r="D2578" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2578" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2579" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2579" t="s">
+        <v>2751</v>
+      </c>
+      <c r="D2579" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2579" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2580" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C2580" t="s">
+        <v>2752</v>
+      </c>
+      <c r="D2580" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2580" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2581" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2581" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2581" t="s">
+        <v>2753</v>
+      </c>
+      <c r="D2581" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2581" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2582" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2582" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C2582" t="s">
+        <v>2754</v>
+      </c>
+      <c r="D2582" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2582" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2583" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2583" t="s">
+        <v>2756</v>
+      </c>
+      <c r="C2583" t="s">
+        <v>2755</v>
+      </c>
+      <c r="D2583" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2583" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2584" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2584" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2584" t="s">
+        <v>2757</v>
+      </c>
+      <c r="D2584" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2584" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2585" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2585" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2585" t="s">
+        <v>2758</v>
+      </c>
+      <c r="D2585" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2585" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2586" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2586" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2586" t="s">
+        <v>2759</v>
+      </c>
+      <c r="D2586" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2586" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2587" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2587" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2587" t="s">
+        <v>2760</v>
+      </c>
+      <c r="D2587" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2587" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2588" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2588" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2588" t="s">
+        <v>2761</v>
+      </c>
+      <c r="D2588" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2588" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2589" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2589" t="s">
+        <v>933</v>
+      </c>
+      <c r="C2589" t="s">
+        <v>2762</v>
+      </c>
+      <c r="D2589" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2589" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2590" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2590" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2590" s="5" t="s">
+        <v>2763</v>
+      </c>
+      <c r="D2590" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2590" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2591" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2591" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C2591" s="5" t="s">
+        <v>2764</v>
+      </c>
+      <c r="D2591" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2591" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2592" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2592" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2592" t="s">
+        <v>2765</v>
+      </c>
+      <c r="D2592" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2592" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2593" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2593" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C2593" t="s">
+        <v>2766</v>
+      </c>
+      <c r="D2593" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2593" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2594" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2594" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2594" s="5" t="s">
+        <v>2768</v>
+      </c>
+      <c r="D2594" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2594" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2595" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2595" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C2595" t="s">
+        <v>2769</v>
+      </c>
+      <c r="D2595" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2595" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2596" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2596" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2596" t="s">
+        <v>2770</v>
+      </c>
+      <c r="D2596" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2596" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2597" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2597" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2597" t="s">
+        <v>2771</v>
+      </c>
+      <c r="D2597" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2597" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2598" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2598" t="s">
+        <v>975</v>
+      </c>
+      <c r="C2598" t="s">
+        <v>2772</v>
+      </c>
+      <c r="D2598" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2598" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2599" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2599" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C2599" s="5" t="s">
+        <v>2773</v>
+      </c>
+      <c r="D2599" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2599" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2600" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2600" t="s">
+        <v>2774</v>
+      </c>
+      <c r="D2600" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2600" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2601" t="s">
+        <v>868</v>
+      </c>
+      <c r="C2601" s="5" t="s">
+        <v>2775</v>
+      </c>
+      <c r="D2601" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2601" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2602" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2602" t="s">
+        <v>2776</v>
+      </c>
+      <c r="D2602" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2602" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2603" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2603" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2603" s="5" t="s">
+        <v>2777</v>
+      </c>
+      <c r="D2603" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2603" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2604" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2604" t="s">
+        <v>2778</v>
+      </c>
+      <c r="D2604" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2604" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2605" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2605" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C2605" t="s">
+        <v>2779</v>
+      </c>
+      <c r="D2605" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2605" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2606" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2606" t="s">
+        <v>577</v>
+      </c>
+      <c r="C2606" s="5" t="s">
+        <v>2780</v>
+      </c>
+      <c r="D2606" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2606" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2607" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2607" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C2607" t="s">
+        <v>2781</v>
+      </c>
+      <c r="D2607" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2607" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2608" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2608" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C2608" t="s">
+        <v>2782</v>
+      </c>
+      <c r="D2608" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2608" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2609" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2609" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C2609" t="s">
+        <v>2783</v>
+      </c>
+      <c r="D2609" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2609" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AZ2527" xr:uid="{0BDF6F9C-D91E-49CF-9ECB-F3D5EC4564BE}"/>
+  <autoFilter ref="A1:AZ2592" xr:uid="{0BDF6F9C-D91E-49CF-9ECB-F3D5EC4564BE}"/>
   <sortState ref="A2:AZ2470">
     <sortCondition ref="A2:A2470"/>
     <sortCondition ref="C2:C2470"/>

</xml_diff>